<commit_message>
Fix typo in sauter mean diameter in niba4 in data_main.xlsx
</commit_message>
<xml_diff>
--- a/Separator Model/Input/data_main.xlsx
+++ b/Separator Model/Input/data_main.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24332"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/bd1a17303fcb2a19/Documentos/RWTH/Semester 4 (SS25)/MA/W14_Modelle_Auswerten/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="T:\public\03 Studenten\00 Ausgeschieden\Ivan Guzman\05_Simulations\Abscheidermodell\MA\MA-Model_4\Separator Model\Input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="79" documentId="11_AD4DB114E441178AC67DF4C99614D368683EDF28" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5CC74E8F-EF7D-4E8E-B38A-2ADEE4F20AFA}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4124941D-3006-43A3-A71F-311403A7681D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="main" sheetId="1" r:id="rId1"/>
@@ -27,8 +27,6 @@
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -114,7 +112,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Standard" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -398,11 +396,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F50"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="B49" sqref="B49"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
@@ -1349,7 +1347,7 @@
         <v>8</v>
       </c>
       <c r="B48">
-        <v>6.3029999999999996E-3</v>
+        <v>6.3029999999999998E-4</v>
       </c>
       <c r="C48">
         <v>1500</v>

</xml_diff>

<commit_message>
Updated data_main.xlsx and parallel excecution code for detail tests.
</commit_message>
<xml_diff>
--- a/Separator Model/Input/data_main.xlsx
+++ b/Separator Model/Input/data_main.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\iagr9\Projekte\MA\MA-Model_4\Separator Model\Input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10055468-AFF3-4FA5-9D37-04ACA1E8EE33}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{001C5818-F282-40CA-8DA0-39B43ED1A302}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-4620" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="main" sheetId="1" r:id="rId1"/>
     <sheet name="sozh" sheetId="2" r:id="rId2"/>
+    <sheet name="detail_V_dis" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="459" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="571" uniqueCount="21">
   <si>
     <t>exp</t>
   </si>
@@ -106,7 +107,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -128,6 +129,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -143,7 +152,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -151,15 +160,31 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -2405,7 +2430,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AE2B3A06-4DE5-48EC-A9CD-6616EFAB12EB}">
   <dimension ref="A1:H363"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A327" workbookViewId="0">
+    <sheetView topLeftCell="A327" workbookViewId="0">
       <selection activeCell="G363" sqref="G363"/>
     </sheetView>
   </sheetViews>
@@ -11855,4 +11880,2749 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{19D26A40-5EC0-4FC2-A7B8-9E1205DD29FB}">
+  <dimension ref="A1:H105"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A69" workbookViewId="0">
+      <selection activeCell="D105" sqref="D105"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="G1" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="H1" s="4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B2">
+        <v>2.0462099999999999E-4</v>
+      </c>
+      <c r="C2">
+        <v>743.10170100000005</v>
+      </c>
+      <c r="D2">
+        <v>0.29701893400000001</v>
+      </c>
+      <c r="E2">
+        <v>3.6502927999999997E-2</v>
+      </c>
+      <c r="F2">
+        <v>9.6633421999999997E-2</v>
+      </c>
+      <c r="G2">
+        <v>4.4652340000000002E-3</v>
+      </c>
+      <c r="H2">
+        <v>0.98750888400000003</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B3">
+        <v>6.5725699999999996E-4</v>
+      </c>
+      <c r="C3">
+        <v>748.36788460000002</v>
+      </c>
+      <c r="D3">
+        <v>0.50333939500000002</v>
+      </c>
+      <c r="E3">
+        <v>2.8484735000000001E-2</v>
+      </c>
+      <c r="F3">
+        <v>9.2660582000000005E-2</v>
+      </c>
+      <c r="G3">
+        <v>1.528742E-3</v>
+      </c>
+      <c r="H3">
+        <v>0.99108918400000001</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>16</v>
+      </c>
+      <c r="B4">
+        <v>3.1127999999999999E-4</v>
+      </c>
+      <c r="C4">
+        <v>749.92972780000002</v>
+      </c>
+      <c r="D4">
+        <v>0.49988101000000001</v>
+      </c>
+      <c r="E4">
+        <v>3.8919571E-2</v>
+      </c>
+      <c r="F4">
+        <v>0.10772396300000001</v>
+      </c>
+      <c r="G4">
+        <v>4.7552549999999999E-3</v>
+      </c>
+      <c r="H4">
+        <v>0.99268671900000005</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>16</v>
+      </c>
+      <c r="B5">
+        <v>4.4927699999999999E-4</v>
+      </c>
+      <c r="C5">
+        <v>749.97402599999998</v>
+      </c>
+      <c r="D5">
+        <v>0.399764919</v>
+      </c>
+      <c r="E5">
+        <v>3.8463404E-2</v>
+      </c>
+      <c r="F5">
+        <v>9.5001253999999993E-2</v>
+      </c>
+      <c r="G5">
+        <v>3.785549E-3</v>
+      </c>
+      <c r="H5">
+        <v>0.98653263199999996</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>17</v>
+      </c>
+      <c r="B6">
+        <v>5.4967899999999997E-4</v>
+      </c>
+      <c r="C6">
+        <v>750.02556879999997</v>
+      </c>
+      <c r="D6">
+        <v>0.50015754999999995</v>
+      </c>
+      <c r="E6">
+        <v>4.0361706999999997E-2</v>
+      </c>
+      <c r="F6">
+        <v>0.101830843</v>
+      </c>
+      <c r="G6">
+        <v>5.2321299999999998E-3</v>
+      </c>
+      <c r="H6">
+        <v>0.99445781600000005</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>16</v>
+      </c>
+      <c r="B7">
+        <v>3.38769E-4</v>
+      </c>
+      <c r="C7">
+        <v>750.05733190000001</v>
+      </c>
+      <c r="D7">
+        <v>0.49989457599999998</v>
+      </c>
+      <c r="E7">
+        <v>3.8023349999999997E-2</v>
+      </c>
+      <c r="F7">
+        <v>0.108397884</v>
+      </c>
+      <c r="G7">
+        <v>4.1389720000000003E-3</v>
+      </c>
+      <c r="H7">
+        <v>0.99176721899999998</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>16</v>
+      </c>
+      <c r="B8">
+        <v>2.4194099999999999E-4</v>
+      </c>
+      <c r="C8">
+        <v>750.20782199999996</v>
+      </c>
+      <c r="D8">
+        <v>0.40002338700000001</v>
+      </c>
+      <c r="E8">
+        <v>6.6916982E-2</v>
+      </c>
+      <c r="F8">
+        <v>0.106790285</v>
+      </c>
+      <c r="G8">
+        <v>5.2340670000000002E-3</v>
+      </c>
+      <c r="H8">
+        <v>0.99171526700000001</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>16</v>
+      </c>
+      <c r="B9">
+        <v>4.9274500000000005E-4</v>
+      </c>
+      <c r="C9">
+        <v>750.25178530000005</v>
+      </c>
+      <c r="D9">
+        <v>0.29988877800000002</v>
+      </c>
+      <c r="E9">
+        <v>3.6448479999999998E-2</v>
+      </c>
+      <c r="F9">
+        <v>0.10019613600000001</v>
+      </c>
+      <c r="G9">
+        <v>2.8000159999999998E-3</v>
+      </c>
+      <c r="H9">
+        <v>0.98938694400000005</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>18</v>
+      </c>
+      <c r="B10">
+        <v>6.1183099999999996E-4</v>
+      </c>
+      <c r="C10">
+        <v>750.71744000000001</v>
+      </c>
+      <c r="D10">
+        <v>0.50033280999999996</v>
+      </c>
+      <c r="E10">
+        <v>3.7521118999999999E-2</v>
+      </c>
+      <c r="F10">
+        <v>9.8495864000000002E-2</v>
+      </c>
+      <c r="G10">
+        <v>3.1483090000000002E-3</v>
+      </c>
+      <c r="H10">
+        <v>0.99218971899999997</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>19</v>
+      </c>
+      <c r="B11">
+        <v>3.9097999999999997E-4</v>
+      </c>
+      <c r="C11">
+        <v>750.86723619999998</v>
+      </c>
+      <c r="D11">
+        <v>0.30092750000000001</v>
+      </c>
+      <c r="E11">
+        <v>3.3229887E-2</v>
+      </c>
+      <c r="F11">
+        <v>0.100884113</v>
+      </c>
+      <c r="G11">
+        <v>3.2887580000000001E-3</v>
+      </c>
+      <c r="H11">
+        <v>0.99199386300000003</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>17</v>
+      </c>
+      <c r="B12">
+        <v>2.2167000000000001E-4</v>
+      </c>
+      <c r="C12">
+        <v>751.48936860000003</v>
+      </c>
+      <c r="D12">
+        <v>0.40003253100000002</v>
+      </c>
+      <c r="E12">
+        <v>7.0955006000000001E-2</v>
+      </c>
+      <c r="F12">
+        <v>0.11041532699999999</v>
+      </c>
+      <c r="G12">
+        <v>4.5576050000000002E-3</v>
+      </c>
+      <c r="H12">
+        <v>0.99505433700000001</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>17</v>
+      </c>
+      <c r="B13">
+        <v>6.7796600000000001E-4</v>
+      </c>
+      <c r="C13">
+        <v>752.85933369999998</v>
+      </c>
+      <c r="D13">
+        <v>0.49949943499999999</v>
+      </c>
+      <c r="E13">
+        <v>4.2382797999999999E-2</v>
+      </c>
+      <c r="F13">
+        <v>9.7580385000000006E-2</v>
+      </c>
+      <c r="G13">
+        <v>3.6210349999999999E-3</v>
+      </c>
+      <c r="H13">
+        <v>0.99436792399999996</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>19</v>
+      </c>
+      <c r="B14">
+        <v>2.54348E-4</v>
+      </c>
+      <c r="C14">
+        <v>908.35374130000002</v>
+      </c>
+      <c r="D14">
+        <v>0.27718706700000001</v>
+      </c>
+      <c r="E14">
+        <v>3.6368708E-2</v>
+      </c>
+      <c r="F14">
+        <v>0.103970942</v>
+      </c>
+      <c r="G14">
+        <v>3.6805710000000001E-3</v>
+      </c>
+      <c r="H14">
+        <v>0.99263151500000002</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>13</v>
+      </c>
+      <c r="B15">
+        <v>8.0239500000000002E-4</v>
+      </c>
+      <c r="C15">
+        <v>998.44373169999994</v>
+      </c>
+      <c r="D15">
+        <v>0.499859416</v>
+      </c>
+      <c r="E15">
+        <v>1.8851822000000001E-2</v>
+      </c>
+      <c r="F15">
+        <v>0.10280117799999999</v>
+      </c>
+      <c r="G15">
+        <v>3.8602500000000002E-4</v>
+      </c>
+      <c r="H15">
+        <v>0.99546705300000005</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>18</v>
+      </c>
+      <c r="B16">
+        <v>5.0275999999999999E-4</v>
+      </c>
+      <c r="C16">
+        <v>999.40820970000004</v>
+      </c>
+      <c r="D16">
+        <v>0.29920427599999999</v>
+      </c>
+      <c r="E16">
+        <v>4.1816536000000001E-2</v>
+      </c>
+      <c r="F16">
+        <v>0.101860464</v>
+      </c>
+      <c r="G16">
+        <v>4.1493759999999998E-3</v>
+      </c>
+      <c r="H16">
+        <v>0.98989876499999996</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>13</v>
+      </c>
+      <c r="B17">
+        <v>5.9944000000000002E-4</v>
+      </c>
+      <c r="C17">
+        <v>999.59662909999997</v>
+      </c>
+      <c r="D17">
+        <v>0.40006547100000001</v>
+      </c>
+      <c r="E17">
+        <v>2.4784075999999999E-2</v>
+      </c>
+      <c r="F17">
+        <v>9.7689174000000004E-2</v>
+      </c>
+      <c r="G17">
+        <v>4.8635799999999999E-4</v>
+      </c>
+      <c r="H17">
+        <v>0.99499302099999998</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>15</v>
+      </c>
+      <c r="B18">
+        <v>7.1244500000000003E-4</v>
+      </c>
+      <c r="C18">
+        <v>999.64467930000001</v>
+      </c>
+      <c r="D18">
+        <v>0.49991358299999999</v>
+      </c>
+      <c r="E18">
+        <v>1.8550810000000001E-2</v>
+      </c>
+      <c r="F18">
+        <v>9.4884389999999999E-2</v>
+      </c>
+      <c r="G18">
+        <v>2.2179650000000001E-3</v>
+      </c>
+      <c r="H18">
+        <v>0.99704778699999996</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>16</v>
+      </c>
+      <c r="B19">
+        <v>3.7785800000000001E-4</v>
+      </c>
+      <c r="C19">
+        <v>999.67359969999995</v>
+      </c>
+      <c r="D19">
+        <v>0.30006925000000001</v>
+      </c>
+      <c r="E19">
+        <v>3.6809690999999999E-2</v>
+      </c>
+      <c r="F19">
+        <v>0.108183192</v>
+      </c>
+      <c r="G19">
+        <v>4.052745E-3</v>
+      </c>
+      <c r="H19">
+        <v>0.98579144299999999</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>15</v>
+      </c>
+      <c r="B20">
+        <v>5.6844399999999998E-4</v>
+      </c>
+      <c r="C20">
+        <v>1000.032227</v>
+      </c>
+      <c r="D20">
+        <v>0.29996158899999997</v>
+      </c>
+      <c r="E20">
+        <v>1.9367124999999999E-2</v>
+      </c>
+      <c r="F20">
+        <v>9.7314092000000005E-2</v>
+      </c>
+      <c r="G20">
+        <v>2.175696E-3</v>
+      </c>
+      <c r="H20">
+        <v>0.995888047</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>19</v>
+      </c>
+      <c r="B21">
+        <v>6.5962200000000001E-4</v>
+      </c>
+      <c r="C21">
+        <v>1000.129858</v>
+      </c>
+      <c r="D21">
+        <v>0.49965211700000001</v>
+      </c>
+      <c r="E21">
+        <v>4.2670694000000002E-2</v>
+      </c>
+      <c r="F21">
+        <v>0.10375522299999999</v>
+      </c>
+      <c r="G21">
+        <v>5.4323920000000003E-3</v>
+      </c>
+      <c r="H21">
+        <v>0.99410157700000001</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>15</v>
+      </c>
+      <c r="B22">
+        <v>7.5361500000000001E-4</v>
+      </c>
+      <c r="C22">
+        <v>1000.183129</v>
+      </c>
+      <c r="D22">
+        <v>0.50001522700000001</v>
+      </c>
+      <c r="E22">
+        <v>1.9893559000000002E-2</v>
+      </c>
+      <c r="F22">
+        <v>9.5239508E-2</v>
+      </c>
+      <c r="G22">
+        <v>2.0156449999999999E-3</v>
+      </c>
+      <c r="H22">
+        <v>0.99718886500000004</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>17</v>
+      </c>
+      <c r="B23">
+        <v>3.65507E-4</v>
+      </c>
+      <c r="C23">
+        <v>1000.201091</v>
+      </c>
+      <c r="D23">
+        <v>0.30000356700000003</v>
+      </c>
+      <c r="E23">
+        <v>5.1118615999999999E-2</v>
+      </c>
+      <c r="F23">
+        <v>0.114449734</v>
+      </c>
+      <c r="G23">
+        <v>4.440495E-3</v>
+      </c>
+      <c r="H23">
+        <v>0.99139601200000005</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>19</v>
+      </c>
+      <c r="B24">
+        <v>3.21902E-4</v>
+      </c>
+      <c r="C24">
+        <v>1000.303949</v>
+      </c>
+      <c r="D24">
+        <v>0.50013415000000006</v>
+      </c>
+      <c r="E24">
+        <v>5.7089112999999997E-2</v>
+      </c>
+      <c r="F24">
+        <v>0.11521322000000001</v>
+      </c>
+      <c r="G24">
+        <v>4.8777610000000004E-3</v>
+      </c>
+      <c r="H24">
+        <v>0.99550441999999995</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>18</v>
+      </c>
+      <c r="B25">
+        <v>4.4690600000000001E-4</v>
+      </c>
+      <c r="C25">
+        <v>1000.564352</v>
+      </c>
+      <c r="D25">
+        <v>0.40118413600000002</v>
+      </c>
+      <c r="E25">
+        <v>4.5435773999999998E-2</v>
+      </c>
+      <c r="F25">
+        <v>0.10055367599999999</v>
+      </c>
+      <c r="G25">
+        <v>4.5400780000000003E-3</v>
+      </c>
+      <c r="H25">
+        <v>0.98875126400000002</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>19</v>
+      </c>
+      <c r="B26">
+        <v>2.6539199999999998E-4</v>
+      </c>
+      <c r="C26">
+        <v>1002.961609</v>
+      </c>
+      <c r="D26">
+        <v>0.30087852900000001</v>
+      </c>
+      <c r="E26">
+        <v>7.5760642000000003E-2</v>
+      </c>
+      <c r="F26">
+        <v>0.10911349100000001</v>
+      </c>
+      <c r="G26">
+        <v>5.1225200000000002E-3</v>
+      </c>
+      <c r="H26">
+        <v>0.99228384400000003</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>17</v>
+      </c>
+      <c r="B27">
+        <v>2.7240599999999999E-4</v>
+      </c>
+      <c r="C27">
+        <v>1242.8563799999999</v>
+      </c>
+      <c r="D27">
+        <v>0.29883443599999998</v>
+      </c>
+      <c r="E27">
+        <v>6.6170259999999995E-2</v>
+      </c>
+      <c r="F27">
+        <v>0.11349644</v>
+      </c>
+      <c r="G27">
+        <v>5.5628220000000003E-3</v>
+      </c>
+      <c r="H27">
+        <v>0.99175836900000003</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>17</v>
+      </c>
+      <c r="B28">
+        <v>5.6636299999999996E-4</v>
+      </c>
+      <c r="C28">
+        <v>1249.038305</v>
+      </c>
+      <c r="D28">
+        <v>0.50009379399999998</v>
+      </c>
+      <c r="E28">
+        <v>5.5513298000000003E-2</v>
+      </c>
+      <c r="F28">
+        <v>0.114298685</v>
+      </c>
+      <c r="G28">
+        <v>5.8367810000000001E-3</v>
+      </c>
+      <c r="H28">
+        <v>0.99043759600000003</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>17</v>
+      </c>
+      <c r="B29">
+        <v>4.4455299999999998E-4</v>
+      </c>
+      <c r="C29">
+        <v>1249.8621929999999</v>
+      </c>
+      <c r="D29">
+        <v>0.29980042600000001</v>
+      </c>
+      <c r="E29">
+        <v>3.1885854999999998E-2</v>
+      </c>
+      <c r="F29">
+        <v>0.10856081200000001</v>
+      </c>
+      <c r="G29">
+        <v>3.8722560000000001E-3</v>
+      </c>
+      <c r="H29">
+        <v>0.98956896599999999</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>16</v>
+      </c>
+      <c r="B30">
+        <v>3.4781999999999999E-4</v>
+      </c>
+      <c r="C30">
+        <v>1249.9720520000001</v>
+      </c>
+      <c r="D30">
+        <v>0.29999618500000003</v>
+      </c>
+      <c r="E30">
+        <v>4.7035642000000003E-2</v>
+      </c>
+      <c r="F30">
+        <v>0.10975439100000001</v>
+      </c>
+      <c r="G30">
+        <v>4.7517119999999999E-3</v>
+      </c>
+      <c r="H30">
+        <v>0.98241363800000003</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>18</v>
+      </c>
+      <c r="B31">
+        <v>3.0862499999999998E-4</v>
+      </c>
+      <c r="C31">
+        <v>1250.009063</v>
+      </c>
+      <c r="D31">
+        <v>0.300016848</v>
+      </c>
+      <c r="E31">
+        <v>4.267257E-2</v>
+      </c>
+      <c r="F31">
+        <v>0.107568497</v>
+      </c>
+      <c r="G31">
+        <v>4.6496790000000003E-3</v>
+      </c>
+      <c r="H31">
+        <v>0.98361751799999997</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>19</v>
+      </c>
+      <c r="B32">
+        <v>3.9580799999999999E-4</v>
+      </c>
+      <c r="C32">
+        <v>1250.0364039999999</v>
+      </c>
+      <c r="D32">
+        <v>0.29999587</v>
+      </c>
+      <c r="E32">
+        <v>4.6113999000000003E-2</v>
+      </c>
+      <c r="F32">
+        <v>0.11548971800000001</v>
+      </c>
+      <c r="G32">
+        <v>4.2850120000000004E-3</v>
+      </c>
+      <c r="H32">
+        <v>0.99005631800000005</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>19</v>
+      </c>
+      <c r="B33">
+        <v>4.85129E-4</v>
+      </c>
+      <c r="C33">
+        <v>1250.056002</v>
+      </c>
+      <c r="D33">
+        <v>0.30007985999999998</v>
+      </c>
+      <c r="E33">
+        <v>3.1432143000000003E-2</v>
+      </c>
+      <c r="F33">
+        <v>0.11381099</v>
+      </c>
+      <c r="G33">
+        <v>4.0394979999999999E-3</v>
+      </c>
+      <c r="H33">
+        <v>0.99273382399999999</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>19</v>
+      </c>
+      <c r="B34">
+        <v>4.7428800000000001E-4</v>
+      </c>
+      <c r="C34">
+        <v>1250.0886849999999</v>
+      </c>
+      <c r="D34">
+        <v>0.30001281800000001</v>
+      </c>
+      <c r="E34">
+        <v>3.3010744000000002E-2</v>
+      </c>
+      <c r="F34">
+        <v>0.11308117199999999</v>
+      </c>
+      <c r="G34">
+        <v>5.2047889999999996E-3</v>
+      </c>
+      <c r="H34">
+        <v>0.99108814999999995</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>17</v>
+      </c>
+      <c r="B35">
+        <v>3.4672300000000001E-4</v>
+      </c>
+      <c r="C35">
+        <v>1250.9434040000001</v>
+      </c>
+      <c r="D35">
+        <v>0.39999618199999998</v>
+      </c>
+      <c r="E35">
+        <v>6.9506928999999995E-2</v>
+      </c>
+      <c r="F35">
+        <v>0.110695898</v>
+      </c>
+      <c r="G35">
+        <v>6.4767380000000001E-3</v>
+      </c>
+      <c r="H35">
+        <v>0.99251876100000003</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>16</v>
+      </c>
+      <c r="B36">
+        <v>5.7827599999999996E-4</v>
+      </c>
+      <c r="C36">
+        <v>1252.670832</v>
+      </c>
+      <c r="D36">
+        <v>0.49995556099999999</v>
+      </c>
+      <c r="E36">
+        <v>4.8558603999999998E-2</v>
+      </c>
+      <c r="F36">
+        <v>9.5985962999999994E-2</v>
+      </c>
+      <c r="G36">
+        <v>5.6972220000000001E-3</v>
+      </c>
+      <c r="H36">
+        <v>0.98525604600000005</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>18</v>
+      </c>
+      <c r="B37">
+        <v>4.6433100000000001E-4</v>
+      </c>
+      <c r="C37">
+        <v>1255.424561</v>
+      </c>
+      <c r="D37">
+        <v>0.39989443400000002</v>
+      </c>
+      <c r="E37">
+        <v>4.1705930000000002E-2</v>
+      </c>
+      <c r="F37">
+        <v>0.10475915299999999</v>
+      </c>
+      <c r="G37">
+        <v>4.4100290000000002E-3</v>
+      </c>
+      <c r="H37">
+        <v>0.98489914300000003</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>17</v>
+      </c>
+      <c r="B38">
+        <v>4.11395E-4</v>
+      </c>
+      <c r="C38">
+        <v>1267.5140690000001</v>
+      </c>
+      <c r="D38">
+        <v>0.49920661399999999</v>
+      </c>
+      <c r="E38">
+        <v>4.8344787E-2</v>
+      </c>
+      <c r="F38">
+        <v>0.12562072899999999</v>
+      </c>
+      <c r="G38">
+        <v>3.9256580000000003E-3</v>
+      </c>
+      <c r="H38">
+        <v>0.99312282299999999</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>17</v>
+      </c>
+      <c r="B39">
+        <v>3.13467E-4</v>
+      </c>
+      <c r="C39">
+        <v>1271.3936630000001</v>
+      </c>
+      <c r="D39">
+        <v>0.40056073800000003</v>
+      </c>
+      <c r="E39">
+        <v>7.1139833E-2</v>
+      </c>
+      <c r="F39">
+        <v>0.11312243299999999</v>
+      </c>
+      <c r="G39">
+        <v>5.9295399999999996E-3</v>
+      </c>
+      <c r="H39">
+        <v>0.99374623100000004</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>15</v>
+      </c>
+      <c r="B40">
+        <v>7.2654800000000004E-4</v>
+      </c>
+      <c r="C40">
+        <v>1455.6305829999999</v>
+      </c>
+      <c r="D40">
+        <v>0.49692148400000002</v>
+      </c>
+      <c r="E40">
+        <v>2.3973168999999999E-2</v>
+      </c>
+      <c r="F40">
+        <v>9.1711663999999998E-2</v>
+      </c>
+      <c r="G40">
+        <v>2.966729E-3</v>
+      </c>
+      <c r="H40">
+        <v>0.99718670099999995</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>15</v>
+      </c>
+      <c r="B41">
+        <v>8.1662800000000002E-4</v>
+      </c>
+      <c r="C41">
+        <v>1492.737848</v>
+      </c>
+      <c r="D41">
+        <v>0.50025813699999999</v>
+      </c>
+      <c r="E41">
+        <v>2.6577284999999999E-2</v>
+      </c>
+      <c r="F41">
+        <v>9.2475197999999995E-2</v>
+      </c>
+      <c r="G41">
+        <v>2.9827109999999999E-3</v>
+      </c>
+      <c r="H41">
+        <v>0.99533773199999998</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>15</v>
+      </c>
+      <c r="B42">
+        <v>8.5975099999999996E-4</v>
+      </c>
+      <c r="C42">
+        <v>1494.673636</v>
+      </c>
+      <c r="D42">
+        <v>0.50000099099999995</v>
+      </c>
+      <c r="E42">
+        <v>2.6915963000000001E-2</v>
+      </c>
+      <c r="F42">
+        <v>9.1934420000000003E-2</v>
+      </c>
+      <c r="G42">
+        <v>2.846627E-3</v>
+      </c>
+      <c r="H42">
+        <v>0.99697522500000002</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>14</v>
+      </c>
+      <c r="B43">
+        <v>7.0617800000000001E-4</v>
+      </c>
+      <c r="C43">
+        <v>1497.1705119999999</v>
+      </c>
+      <c r="D43">
+        <v>0.49990232400000001</v>
+      </c>
+      <c r="E43">
+        <v>2.4668497000000001E-2</v>
+      </c>
+      <c r="F43">
+        <v>9.1588153000000005E-2</v>
+      </c>
+      <c r="G43">
+        <v>3.0430520000000001E-3</v>
+      </c>
+      <c r="H43">
+        <v>0.99707969600000002</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>13</v>
+      </c>
+      <c r="B44">
+        <v>6.3737199999999998E-4</v>
+      </c>
+      <c r="C44">
+        <v>1500.051467</v>
+      </c>
+      <c r="D44">
+        <v>0.29994249899999997</v>
+      </c>
+      <c r="E44">
+        <v>2.6047677000000002E-2</v>
+      </c>
+      <c r="F44">
+        <v>0.10857765</v>
+      </c>
+      <c r="G44">
+        <v>7.1048200000000002E-4</v>
+      </c>
+      <c r="H44">
+        <v>0.99349073799999998</v>
+      </c>
+    </row>
+    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>15</v>
+      </c>
+      <c r="B45">
+        <v>5.2616900000000005E-4</v>
+      </c>
+      <c r="C45">
+        <v>1500.0874120000001</v>
+      </c>
+      <c r="D45">
+        <v>0.30007125099999998</v>
+      </c>
+      <c r="E45">
+        <v>1.9110674000000001E-2</v>
+      </c>
+      <c r="F45">
+        <v>0.12915310899999999</v>
+      </c>
+      <c r="G45">
+        <v>7.8471699999999999E-4</v>
+      </c>
+      <c r="H45">
+        <v>0.99525415699999997</v>
+      </c>
+    </row>
+    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>13</v>
+      </c>
+      <c r="B46">
+        <v>7.4180700000000003E-4</v>
+      </c>
+      <c r="C46">
+        <v>1500.215265</v>
+      </c>
+      <c r="D46">
+        <v>0.39993976599999997</v>
+      </c>
+      <c r="E46">
+        <v>2.7369943000000001E-2</v>
+      </c>
+      <c r="F46">
+        <v>9.7766817000000006E-2</v>
+      </c>
+      <c r="G46">
+        <v>4.3964299999999998E-4</v>
+      </c>
+      <c r="H46">
+        <v>0.99480906899999999</v>
+      </c>
+    </row>
+    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>13</v>
+      </c>
+      <c r="B47">
+        <v>9.1292700000000001E-4</v>
+      </c>
+      <c r="C47">
+        <v>1500.5413000000001</v>
+      </c>
+      <c r="D47">
+        <v>0.50044513199999996</v>
+      </c>
+      <c r="E47">
+        <v>2.0620128000000001E-2</v>
+      </c>
+      <c r="F47">
+        <v>0.103834646</v>
+      </c>
+      <c r="G47">
+        <v>4.4096199999999998E-4</v>
+      </c>
+      <c r="H47">
+        <v>0.99445706499999997</v>
+      </c>
+    </row>
+    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>13</v>
+      </c>
+      <c r="B48">
+        <v>9.4360899999999998E-4</v>
+      </c>
+      <c r="C48">
+        <v>1500.993866</v>
+      </c>
+      <c r="D48">
+        <v>0.499986655</v>
+      </c>
+      <c r="E48">
+        <v>2.1720821000000001E-2</v>
+      </c>
+      <c r="F48">
+        <v>0.103615651</v>
+      </c>
+      <c r="G48">
+        <v>8.3131500000000001E-4</v>
+      </c>
+      <c r="H48">
+        <v>0.99464200000000003</v>
+      </c>
+    </row>
+    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>15</v>
+      </c>
+      <c r="B49">
+        <v>6.1466400000000001E-4</v>
+      </c>
+      <c r="C49">
+        <v>1502.4972680000001</v>
+      </c>
+      <c r="D49">
+        <v>0.40017336999999997</v>
+      </c>
+      <c r="E49">
+        <v>2.0735538000000001E-2</v>
+      </c>
+      <c r="F49">
+        <v>9.4777095000000006E-2</v>
+      </c>
+      <c r="G49">
+        <v>2.47956E-3</v>
+      </c>
+      <c r="H49">
+        <v>0.99691817900000002</v>
+      </c>
+    </row>
+    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>15</v>
+      </c>
+      <c r="B50">
+        <v>6.6162899999999995E-4</v>
+      </c>
+      <c r="C50">
+        <v>1504.5464079999999</v>
+      </c>
+      <c r="D50">
+        <v>0.40074769799999999</v>
+      </c>
+      <c r="E50">
+        <v>2.2464746000000001E-2</v>
+      </c>
+      <c r="F50">
+        <v>9.4852504000000004E-2</v>
+      </c>
+      <c r="G50">
+        <v>2.9607710000000001E-3</v>
+      </c>
+      <c r="H50">
+        <v>0.99641502000000004</v>
+      </c>
+    </row>
+    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>15</v>
+      </c>
+      <c r="B51">
+        <v>7.2370699999999997E-4</v>
+      </c>
+      <c r="C51">
+        <v>1752.5926159999999</v>
+      </c>
+      <c r="D51">
+        <v>0.50002069100000002</v>
+      </c>
+      <c r="E51">
+        <v>2.4334100000000001E-2</v>
+      </c>
+      <c r="F51">
+        <v>9.0262732999999998E-2</v>
+      </c>
+      <c r="G51">
+        <v>2.7651020000000002E-3</v>
+      </c>
+      <c r="H51">
+        <v>0.99688110399999996</v>
+      </c>
+    </row>
+    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
+        <v>13</v>
+      </c>
+      <c r="B52">
+        <v>8.0128199999999995E-4</v>
+      </c>
+      <c r="C52">
+        <v>1995.9935250000001</v>
+      </c>
+      <c r="D52">
+        <v>0.49970003499999999</v>
+      </c>
+      <c r="E52">
+        <v>2.3888031000000001E-2</v>
+      </c>
+      <c r="F52">
+        <v>0.101849986</v>
+      </c>
+      <c r="G52">
+        <v>6.1271999999999997E-4</v>
+      </c>
+      <c r="H52">
+        <v>0.99330616800000004</v>
+      </c>
+    </row>
+    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
+        <v>15</v>
+      </c>
+      <c r="B53">
+        <v>6.8117199999999996E-4</v>
+      </c>
+      <c r="C53">
+        <v>1999.6194820000001</v>
+      </c>
+      <c r="D53">
+        <v>0.49998881699999997</v>
+      </c>
+      <c r="E53">
+        <v>2.6883537999999998E-2</v>
+      </c>
+      <c r="F53">
+        <v>8.8787929000000002E-2</v>
+      </c>
+      <c r="G53">
+        <v>2.7722139999999998E-3</v>
+      </c>
+      <c r="H53">
+        <v>0.99639685600000005</v>
+      </c>
+    </row>
+    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
+        <v>15</v>
+      </c>
+      <c r="B54">
+        <v>6.1575900000000001E-4</v>
+      </c>
+      <c r="C54">
+        <v>1999.9767119999999</v>
+      </c>
+      <c r="D54">
+        <v>0.40001579300000001</v>
+      </c>
+      <c r="E54">
+        <v>2.3810701E-2</v>
+      </c>
+      <c r="F54">
+        <v>9.3052383000000002E-2</v>
+      </c>
+      <c r="G54">
+        <v>1.4778720000000001E-3</v>
+      </c>
+      <c r="H54">
+        <v>0.99505876199999999</v>
+      </c>
+    </row>
+    <row r="55" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
+        <v>15</v>
+      </c>
+      <c r="B55">
+        <v>5.7284199999999995E-4</v>
+      </c>
+      <c r="C55">
+        <v>2000.4061589999999</v>
+      </c>
+      <c r="D55">
+        <v>0.40002267499999999</v>
+      </c>
+      <c r="E55">
+        <v>2.5438157999999999E-2</v>
+      </c>
+      <c r="F55">
+        <v>8.9342075000000007E-2</v>
+      </c>
+      <c r="G55">
+        <v>1.5362749999999999E-3</v>
+      </c>
+      <c r="H55">
+        <v>0.99545406299999994</v>
+      </c>
+    </row>
+    <row r="56" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
+        <v>14</v>
+      </c>
+      <c r="B56">
+        <v>7.3430900000000005E-4</v>
+      </c>
+      <c r="C56">
+        <v>2000.6603399999999</v>
+      </c>
+      <c r="D56">
+        <v>0.50012684799999996</v>
+      </c>
+      <c r="E56">
+        <v>2.6662858000000001E-2</v>
+      </c>
+      <c r="F56">
+        <v>8.9674559000000001E-2</v>
+      </c>
+      <c r="G56">
+        <v>3.0504239999999999E-3</v>
+      </c>
+      <c r="H56">
+        <v>0.99543250999999999</v>
+      </c>
+    </row>
+    <row r="57" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
+        <v>3</v>
+      </c>
+      <c r="B57">
+        <v>2.5999999999999998E-4</v>
+      </c>
+      <c r="C57">
+        <v>160</v>
+      </c>
+      <c r="D57">
+        <v>0.2</v>
+      </c>
+      <c r="E57">
+        <v>0</v>
+      </c>
+      <c r="F57">
+        <v>0</v>
+      </c>
+      <c r="G57">
+        <v>9.6295699999999996E-4</v>
+      </c>
+      <c r="H57">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="58" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A58" t="s">
+        <v>3</v>
+      </c>
+      <c r="B58">
+        <v>2.81E-4</v>
+      </c>
+      <c r="C58">
+        <v>160</v>
+      </c>
+      <c r="D58">
+        <v>0.2</v>
+      </c>
+      <c r="E58">
+        <v>0</v>
+      </c>
+      <c r="F58">
+        <v>0</v>
+      </c>
+      <c r="G58">
+        <v>5.4068499999999995E-4</v>
+      </c>
+      <c r="H58">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="59" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A59" t="s">
+        <v>3</v>
+      </c>
+      <c r="B59">
+        <v>3.0699999999999998E-4</v>
+      </c>
+      <c r="C59">
+        <v>160</v>
+      </c>
+      <c r="D59">
+        <v>0.2</v>
+      </c>
+      <c r="E59">
+        <v>0</v>
+      </c>
+      <c r="F59">
+        <v>0</v>
+      </c>
+      <c r="G59">
+        <v>5.7356200000000001E-4</v>
+      </c>
+      <c r="H59">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="60" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A60" t="s">
+        <v>3</v>
+      </c>
+      <c r="B60">
+        <v>3.6999999999999999E-4</v>
+      </c>
+      <c r="C60">
+        <v>160</v>
+      </c>
+      <c r="D60">
+        <v>0.2</v>
+      </c>
+      <c r="E60">
+        <v>0</v>
+      </c>
+      <c r="F60">
+        <v>0</v>
+      </c>
+      <c r="G60">
+        <v>1.609114E-3</v>
+      </c>
+      <c r="H60">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="61" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A61" t="s">
+        <v>3</v>
+      </c>
+      <c r="B61">
+        <v>4.3100000000000001E-4</v>
+      </c>
+      <c r="C61">
+        <v>160</v>
+      </c>
+      <c r="D61">
+        <v>0.2</v>
+      </c>
+      <c r="E61">
+        <v>0</v>
+      </c>
+      <c r="F61">
+        <v>0</v>
+      </c>
+      <c r="G61">
+        <v>2.0221039999999998E-3</v>
+      </c>
+      <c r="H61">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="62" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A62" t="s">
+        <v>3</v>
+      </c>
+      <c r="B62">
+        <v>5.3200000000000003E-4</v>
+      </c>
+      <c r="C62">
+        <v>160</v>
+      </c>
+      <c r="D62">
+        <v>0.2</v>
+      </c>
+      <c r="E62">
+        <v>0</v>
+      </c>
+      <c r="F62">
+        <v>0</v>
+      </c>
+      <c r="G62">
+        <v>1.858317E-3</v>
+      </c>
+      <c r="H62">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="63" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A63" t="s">
+        <v>3</v>
+      </c>
+      <c r="B63">
+        <v>6.8900000000000005E-4</v>
+      </c>
+      <c r="C63">
+        <v>160</v>
+      </c>
+      <c r="D63">
+        <v>0.2</v>
+      </c>
+      <c r="E63">
+        <v>0</v>
+      </c>
+      <c r="F63">
+        <v>0</v>
+      </c>
+      <c r="G63">
+        <v>1.541461E-3</v>
+      </c>
+      <c r="H63">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="64" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A64" t="s">
+        <v>3</v>
+      </c>
+      <c r="B64">
+        <v>1.281E-3</v>
+      </c>
+      <c r="C64">
+        <v>160</v>
+      </c>
+      <c r="D64">
+        <v>0.2</v>
+      </c>
+      <c r="E64">
+        <v>0</v>
+      </c>
+      <c r="F64">
+        <v>0</v>
+      </c>
+      <c r="G64">
+        <v>1.2030529999999999E-3</v>
+      </c>
+      <c r="H64">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="65" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A65" t="s">
+        <v>3</v>
+      </c>
+      <c r="B65">
+        <v>2.52E-4</v>
+      </c>
+      <c r="C65">
+        <v>200</v>
+      </c>
+      <c r="D65">
+        <v>0.2</v>
+      </c>
+      <c r="E65">
+        <v>0</v>
+      </c>
+      <c r="F65">
+        <v>0</v>
+      </c>
+      <c r="G65">
+        <v>2.27729E-4</v>
+      </c>
+      <c r="H65">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="66" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A66" t="s">
+        <v>3</v>
+      </c>
+      <c r="B66">
+        <v>2.8299999999999999E-4</v>
+      </c>
+      <c r="C66">
+        <v>200</v>
+      </c>
+      <c r="D66">
+        <v>0.2</v>
+      </c>
+      <c r="E66">
+        <v>0</v>
+      </c>
+      <c r="F66">
+        <v>0</v>
+      </c>
+      <c r="G66">
+        <v>1.347741E-3</v>
+      </c>
+      <c r="H66">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="67" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A67" t="s">
+        <v>3</v>
+      </c>
+      <c r="B67">
+        <v>3.2499999999999999E-4</v>
+      </c>
+      <c r="C67">
+        <v>200</v>
+      </c>
+      <c r="D67">
+        <v>0.2</v>
+      </c>
+      <c r="E67">
+        <v>0</v>
+      </c>
+      <c r="F67">
+        <v>0</v>
+      </c>
+      <c r="G67">
+        <v>1.48168E-3</v>
+      </c>
+      <c r="H67">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="68" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A68" t="s">
+        <v>3</v>
+      </c>
+      <c r="B68">
+        <v>3.8299999999999999E-4</v>
+      </c>
+      <c r="C68">
+        <v>200</v>
+      </c>
+      <c r="D68">
+        <v>0.2</v>
+      </c>
+      <c r="E68">
+        <v>0</v>
+      </c>
+      <c r="F68">
+        <v>0</v>
+      </c>
+      <c r="G68">
+        <v>1.5823530000000001E-3</v>
+      </c>
+      <c r="H68">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="69" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A69" t="s">
+        <v>3</v>
+      </c>
+      <c r="B69">
+        <v>4.64E-4</v>
+      </c>
+      <c r="C69">
+        <v>200</v>
+      </c>
+      <c r="D69">
+        <v>0.2</v>
+      </c>
+      <c r="E69">
+        <v>0</v>
+      </c>
+      <c r="F69">
+        <v>0</v>
+      </c>
+      <c r="G69">
+        <v>1.264077E-3</v>
+      </c>
+      <c r="H69">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="70" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A70" t="s">
+        <v>3</v>
+      </c>
+      <c r="B70">
+        <v>5.8399999999999999E-4</v>
+      </c>
+      <c r="C70">
+        <v>200</v>
+      </c>
+      <c r="D70">
+        <v>0.2</v>
+      </c>
+      <c r="E70">
+        <v>0</v>
+      </c>
+      <c r="F70">
+        <v>0</v>
+      </c>
+      <c r="G70">
+        <v>1.7501089999999999E-3</v>
+      </c>
+      <c r="H70">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="71" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A71" t="s">
+        <v>3</v>
+      </c>
+      <c r="B71">
+        <v>7.8799999999999996E-4</v>
+      </c>
+      <c r="C71">
+        <v>200</v>
+      </c>
+      <c r="D71">
+        <v>0.2</v>
+      </c>
+      <c r="E71">
+        <v>0</v>
+      </c>
+      <c r="F71">
+        <v>0</v>
+      </c>
+      <c r="G71">
+        <v>1.2385709999999999E-3</v>
+      </c>
+      <c r="H71">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="72" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A72" t="s">
+        <v>3</v>
+      </c>
+      <c r="B72">
+        <v>1.0950000000000001E-3</v>
+      </c>
+      <c r="C72">
+        <v>200</v>
+      </c>
+      <c r="D72">
+        <v>0.2</v>
+      </c>
+      <c r="E72">
+        <v>0</v>
+      </c>
+      <c r="F72">
+        <v>0</v>
+      </c>
+      <c r="G72">
+        <v>9.1166800000000003E-4</v>
+      </c>
+      <c r="H72">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="73" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A73" t="s">
+        <v>3</v>
+      </c>
+      <c r="B73">
+        <v>1.5E-3</v>
+      </c>
+      <c r="C73">
+        <v>200</v>
+      </c>
+      <c r="D73">
+        <v>0.2</v>
+      </c>
+      <c r="E73">
+        <v>0</v>
+      </c>
+      <c r="F73">
+        <v>0</v>
+      </c>
+      <c r="G73">
+        <v>4.5693399999999999E-4</v>
+      </c>
+      <c r="H73">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="74" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A74" t="s">
+        <v>3</v>
+      </c>
+      <c r="B74">
+        <v>2.7099999999999997E-4</v>
+      </c>
+      <c r="C74">
+        <v>240</v>
+      </c>
+      <c r="D74">
+        <v>0.2</v>
+      </c>
+      <c r="E74">
+        <v>0</v>
+      </c>
+      <c r="F74">
+        <v>0</v>
+      </c>
+      <c r="G74">
+        <v>5.6943599999999999E-4</v>
+      </c>
+      <c r="H74">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="75" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A75" t="s">
+        <v>3</v>
+      </c>
+      <c r="B75">
+        <v>2.9799999999999998E-4</v>
+      </c>
+      <c r="C75">
+        <v>240</v>
+      </c>
+      <c r="D75">
+        <v>0.2</v>
+      </c>
+      <c r="E75">
+        <v>0</v>
+      </c>
+      <c r="F75">
+        <v>0</v>
+      </c>
+      <c r="G75">
+        <v>1.764112E-3</v>
+      </c>
+      <c r="H75">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="76" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A76" t="s">
+        <v>3</v>
+      </c>
+      <c r="B76">
+        <v>3.4299999999999999E-4</v>
+      </c>
+      <c r="C76">
+        <v>240</v>
+      </c>
+      <c r="D76">
+        <v>0.2</v>
+      </c>
+      <c r="E76">
+        <v>0</v>
+      </c>
+      <c r="F76">
+        <v>0</v>
+      </c>
+      <c r="G76">
+        <v>2.7815829999999998E-3</v>
+      </c>
+      <c r="H76">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="77" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A77" t="s">
+        <v>3</v>
+      </c>
+      <c r="B77">
+        <v>4.0400000000000001E-4</v>
+      </c>
+      <c r="C77">
+        <v>240</v>
+      </c>
+      <c r="D77">
+        <v>0.2</v>
+      </c>
+      <c r="E77">
+        <v>0</v>
+      </c>
+      <c r="F77">
+        <v>0</v>
+      </c>
+      <c r="G77">
+        <v>3.124384E-3</v>
+      </c>
+      <c r="H77">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="78" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A78" t="s">
+        <v>3</v>
+      </c>
+      <c r="B78">
+        <v>5.0299999999999997E-4</v>
+      </c>
+      <c r="C78">
+        <v>240</v>
+      </c>
+      <c r="D78">
+        <v>0.2</v>
+      </c>
+      <c r="E78">
+        <v>0</v>
+      </c>
+      <c r="F78">
+        <v>0</v>
+      </c>
+      <c r="G78">
+        <v>3.5047860000000002E-3</v>
+      </c>
+      <c r="H78">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="79" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A79" t="s">
+        <v>3</v>
+      </c>
+      <c r="B79">
+        <v>6.0999999999999997E-4</v>
+      </c>
+      <c r="C79">
+        <v>240</v>
+      </c>
+      <c r="D79">
+        <v>0.2</v>
+      </c>
+      <c r="E79">
+        <v>0</v>
+      </c>
+      <c r="F79">
+        <v>0</v>
+      </c>
+      <c r="G79">
+        <v>3.015471E-3</v>
+      </c>
+      <c r="H79">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="80" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A80" t="s">
+        <v>3</v>
+      </c>
+      <c r="B80">
+        <v>8.0400000000000003E-4</v>
+      </c>
+      <c r="C80">
+        <v>240</v>
+      </c>
+      <c r="D80">
+        <v>0.2</v>
+      </c>
+      <c r="E80">
+        <v>0</v>
+      </c>
+      <c r="F80">
+        <v>0</v>
+      </c>
+      <c r="G80">
+        <v>2.3056370000000001E-3</v>
+      </c>
+      <c r="H80">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="81" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A81" t="s">
+        <v>3</v>
+      </c>
+      <c r="B81">
+        <v>1.0920000000000001E-3</v>
+      </c>
+      <c r="C81">
+        <v>240</v>
+      </c>
+      <c r="D81">
+        <v>0.2</v>
+      </c>
+      <c r="E81">
+        <v>0</v>
+      </c>
+      <c r="F81">
+        <v>0</v>
+      </c>
+      <c r="G81">
+        <v>1.8617429999999999E-3</v>
+      </c>
+      <c r="H81">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="82" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A82" t="s">
+        <v>3</v>
+      </c>
+      <c r="B82">
+        <v>1.4159999999999999E-3</v>
+      </c>
+      <c r="C82">
+        <v>240</v>
+      </c>
+      <c r="D82">
+        <v>0.2</v>
+      </c>
+      <c r="E82">
+        <v>0</v>
+      </c>
+      <c r="F82">
+        <v>0</v>
+      </c>
+      <c r="G82">
+        <v>9.7170399999999999E-4</v>
+      </c>
+      <c r="H82">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="83" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A83" t="s">
+        <v>3</v>
+      </c>
+      <c r="B83">
+        <v>2.5399999999999999E-4</v>
+      </c>
+      <c r="C83">
+        <v>280</v>
+      </c>
+      <c r="D83">
+        <v>0.2</v>
+      </c>
+      <c r="E83">
+        <v>0</v>
+      </c>
+      <c r="F83">
+        <v>0</v>
+      </c>
+      <c r="G83">
+        <v>6.6906099999999998E-4</v>
+      </c>
+      <c r="H83">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="84" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A84" t="s">
+        <v>3</v>
+      </c>
+      <c r="B84">
+        <v>2.9399999999999999E-4</v>
+      </c>
+      <c r="C84">
+        <v>280</v>
+      </c>
+      <c r="D84">
+        <v>0.2</v>
+      </c>
+      <c r="E84">
+        <v>0</v>
+      </c>
+      <c r="F84">
+        <v>0</v>
+      </c>
+      <c r="G84">
+        <v>2.4819130000000001E-3</v>
+      </c>
+      <c r="H84">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="85" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A85" t="s">
+        <v>3</v>
+      </c>
+      <c r="B85">
+        <v>3.3700000000000001E-4</v>
+      </c>
+      <c r="C85">
+        <v>280</v>
+      </c>
+      <c r="D85">
+        <v>0.2</v>
+      </c>
+      <c r="E85">
+        <v>0</v>
+      </c>
+      <c r="F85">
+        <v>0</v>
+      </c>
+      <c r="G85">
+        <v>3.5047860000000002E-3</v>
+      </c>
+      <c r="H85">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="86" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A86" t="s">
+        <v>3</v>
+      </c>
+      <c r="B86">
+        <v>4.0200000000000001E-4</v>
+      </c>
+      <c r="C86">
+        <v>280</v>
+      </c>
+      <c r="D86">
+        <v>0.2</v>
+      </c>
+      <c r="E86">
+        <v>0</v>
+      </c>
+      <c r="F86">
+        <v>0</v>
+      </c>
+      <c r="G86">
+        <v>3.5300269999999998E-3</v>
+      </c>
+      <c r="H86">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="87" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A87" t="s">
+        <v>3</v>
+      </c>
+      <c r="B87">
+        <v>4.9700000000000005E-4</v>
+      </c>
+      <c r="C87">
+        <v>280</v>
+      </c>
+      <c r="D87">
+        <v>0.2</v>
+      </c>
+      <c r="E87">
+        <v>0</v>
+      </c>
+      <c r="F87">
+        <v>0</v>
+      </c>
+      <c r="G87">
+        <v>3.7511160000000001E-3</v>
+      </c>
+      <c r="H87">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="88" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A88" t="s">
+        <v>3</v>
+      </c>
+      <c r="B88">
+        <v>6.1700000000000004E-4</v>
+      </c>
+      <c r="C88">
+        <v>280</v>
+      </c>
+      <c r="D88">
+        <v>0.2</v>
+      </c>
+      <c r="E88">
+        <v>0</v>
+      </c>
+      <c r="F88">
+        <v>0</v>
+      </c>
+      <c r="G88">
+        <v>3.7918209999999999E-3</v>
+      </c>
+      <c r="H88">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="89" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A89" t="s">
+        <v>3</v>
+      </c>
+      <c r="B89">
+        <v>8.0000000000000004E-4</v>
+      </c>
+      <c r="C89">
+        <v>280</v>
+      </c>
+      <c r="D89">
+        <v>0.2</v>
+      </c>
+      <c r="E89">
+        <v>0</v>
+      </c>
+      <c r="F89">
+        <v>0</v>
+      </c>
+      <c r="G89">
+        <v>2.9280959999999998E-3</v>
+      </c>
+      <c r="H89">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="90" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A90" t="s">
+        <v>3</v>
+      </c>
+      <c r="B90">
+        <v>1.0989999999999999E-3</v>
+      </c>
+      <c r="C90">
+        <v>280</v>
+      </c>
+      <c r="D90">
+        <v>0.2</v>
+      </c>
+      <c r="E90">
+        <v>0</v>
+      </c>
+      <c r="F90">
+        <v>0</v>
+      </c>
+      <c r="G90">
+        <v>2.4002030000000001E-3</v>
+      </c>
+      <c r="H90">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="91" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A91" t="s">
+        <v>3</v>
+      </c>
+      <c r="B91">
+        <v>1.2780000000000001E-3</v>
+      </c>
+      <c r="C91">
+        <v>280</v>
+      </c>
+      <c r="D91">
+        <v>0.2</v>
+      </c>
+      <c r="E91">
+        <v>0</v>
+      </c>
+      <c r="F91">
+        <v>0</v>
+      </c>
+      <c r="G91">
+        <v>1.534342E-3</v>
+      </c>
+      <c r="H91">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="92" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A92" t="s">
+        <v>5</v>
+      </c>
+      <c r="B92">
+        <v>6.9999999999999999E-4</v>
+      </c>
+      <c r="C92">
+        <v>2050</v>
+      </c>
+      <c r="D92">
+        <v>0.3</v>
+      </c>
+      <c r="E92">
+        <v>0</v>
+      </c>
+      <c r="F92">
+        <v>0</v>
+      </c>
+      <c r="G92">
+        <v>5.9087439999999996E-3</v>
+      </c>
+      <c r="H92">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="93" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A93" t="s">
+        <v>5</v>
+      </c>
+      <c r="B93">
+        <v>9.0499999999999999E-4</v>
+      </c>
+      <c r="C93">
+        <v>2350</v>
+      </c>
+      <c r="D93">
+        <v>0.5</v>
+      </c>
+      <c r="E93">
+        <v>0</v>
+      </c>
+      <c r="F93">
+        <v>0</v>
+      </c>
+      <c r="G93">
+        <v>5.9087439999999996E-3</v>
+      </c>
+      <c r="H93">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="94" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A94" t="s">
+        <v>6</v>
+      </c>
+      <c r="B94">
+        <v>6.3250000000000003E-4</v>
+      </c>
+      <c r="C94">
+        <v>1600</v>
+      </c>
+      <c r="D94">
+        <v>0.3</v>
+      </c>
+      <c r="E94">
+        <v>0</v>
+      </c>
+      <c r="F94">
+        <v>0</v>
+      </c>
+      <c r="G94">
+        <v>5.9087439999999996E-3</v>
+      </c>
+      <c r="H94">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="95" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A95" t="s">
+        <v>6</v>
+      </c>
+      <c r="B95">
+        <v>6.0749999999999997E-4</v>
+      </c>
+      <c r="C95">
+        <v>1500</v>
+      </c>
+      <c r="D95">
+        <v>0.3</v>
+      </c>
+      <c r="E95">
+        <v>0</v>
+      </c>
+      <c r="F95">
+        <v>0</v>
+      </c>
+      <c r="G95">
+        <v>5.9087439999999996E-3</v>
+      </c>
+      <c r="H95">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="96" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A96" t="s">
+        <v>6</v>
+      </c>
+      <c r="B96">
+        <v>7.3800000000000005E-4</v>
+      </c>
+      <c r="C96">
+        <v>1450</v>
+      </c>
+      <c r="D96">
+        <v>0.5</v>
+      </c>
+      <c r="E96">
+        <v>0</v>
+      </c>
+      <c r="F96">
+        <v>0</v>
+      </c>
+      <c r="G96">
+        <v>5.9087439999999996E-3</v>
+      </c>
+      <c r="H96">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="97" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A97" t="s">
+        <v>6</v>
+      </c>
+      <c r="B97">
+        <v>8.6499999999999999E-4</v>
+      </c>
+      <c r="C97">
+        <v>1850</v>
+      </c>
+      <c r="D97">
+        <v>0.5</v>
+      </c>
+      <c r="E97">
+        <v>0</v>
+      </c>
+      <c r="F97">
+        <v>0</v>
+      </c>
+      <c r="G97">
+        <v>5.9087439999999996E-3</v>
+      </c>
+      <c r="H97">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="98" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A98" t="s">
+        <v>7</v>
+      </c>
+      <c r="B98">
+        <v>6.2750000000000002E-4</v>
+      </c>
+      <c r="C98">
+        <v>1600</v>
+      </c>
+      <c r="D98">
+        <v>0.3</v>
+      </c>
+      <c r="E98">
+        <v>0</v>
+      </c>
+      <c r="F98">
+        <v>0</v>
+      </c>
+      <c r="G98">
+        <v>5.9087439999999996E-3</v>
+      </c>
+      <c r="H98">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="99" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A99" t="s">
+        <v>7</v>
+      </c>
+      <c r="B99">
+        <v>5.8500000000000002E-4</v>
+      </c>
+      <c r="C99">
+        <v>1450</v>
+      </c>
+      <c r="D99">
+        <v>0.3</v>
+      </c>
+      <c r="E99">
+        <v>0</v>
+      </c>
+      <c r="F99">
+        <v>0</v>
+      </c>
+      <c r="G99">
+        <v>5.9087439999999996E-3</v>
+      </c>
+      <c r="H99">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="100" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A100" t="s">
+        <v>7</v>
+      </c>
+      <c r="B100">
+        <v>7.0750000000000001E-4</v>
+      </c>
+      <c r="C100">
+        <v>1400</v>
+      </c>
+      <c r="D100">
+        <v>0.5</v>
+      </c>
+      <c r="E100">
+        <v>0</v>
+      </c>
+      <c r="F100">
+        <v>0</v>
+      </c>
+      <c r="G100">
+        <v>5.9087439999999996E-3</v>
+      </c>
+      <c r="H100">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="101" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A101" t="s">
+        <v>7</v>
+      </c>
+      <c r="B101">
+        <v>6.3500000000000004E-4</v>
+      </c>
+      <c r="C101">
+        <v>1150</v>
+      </c>
+      <c r="D101">
+        <v>0.5</v>
+      </c>
+      <c r="E101">
+        <v>0</v>
+      </c>
+      <c r="F101">
+        <v>0</v>
+      </c>
+      <c r="G101">
+        <v>5.9087439999999996E-3</v>
+      </c>
+      <c r="H101">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="102" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A102" t="s">
+        <v>8</v>
+      </c>
+      <c r="B102">
+        <v>6.6750000000000002E-4</v>
+      </c>
+      <c r="C102">
+        <v>1600</v>
+      </c>
+      <c r="D102">
+        <v>0.3</v>
+      </c>
+      <c r="E102">
+        <v>0</v>
+      </c>
+      <c r="F102">
+        <v>0</v>
+      </c>
+      <c r="G102">
+        <v>5.9087439999999996E-3</v>
+      </c>
+      <c r="H102">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="103" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A103" t="s">
+        <v>8</v>
+      </c>
+      <c r="B103">
+        <v>6.3029999999999998E-4</v>
+      </c>
+      <c r="C103">
+        <v>1500</v>
+      </c>
+      <c r="D103">
+        <v>0.3</v>
+      </c>
+      <c r="E103">
+        <v>0</v>
+      </c>
+      <c r="F103">
+        <v>0</v>
+      </c>
+      <c r="G103">
+        <v>5.9087439999999996E-3</v>
+      </c>
+      <c r="H103">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="104" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A104" t="s">
+        <v>8</v>
+      </c>
+      <c r="B104">
+        <v>7.2250000000000005E-4</v>
+      </c>
+      <c r="C104">
+        <v>1350</v>
+      </c>
+      <c r="D104">
+        <v>0.5</v>
+      </c>
+      <c r="E104">
+        <v>0</v>
+      </c>
+      <c r="F104">
+        <v>0</v>
+      </c>
+      <c r="G104">
+        <v>5.9087439999999996E-3</v>
+      </c>
+      <c r="H104">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="105" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A105" t="s">
+        <v>8</v>
+      </c>
+      <c r="B105">
+        <v>6.7250000000000003E-4</v>
+      </c>
+      <c r="C105">
+        <v>1200</v>
+      </c>
+      <c r="D105">
+        <v>0.5</v>
+      </c>
+      <c r="E105">
+        <v>0</v>
+      </c>
+      <c r="F105">
+        <v>0</v>
+      </c>
+      <c r="G105">
+        <v>5.9087439999999996E-3</v>
+      </c>
+      <c r="H105">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Updated parallel code for running lambda detail tests. Also added lamdda detail sheet to data_main.xlsx in the Input folder.
</commit_message>
<xml_diff>
--- a/Separator Model/Input/data_main.xlsx
+++ b/Separator Model/Input/data_main.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\iagr9\Projekte\MA\MA-Model_4\Separator Model\Input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{001C5818-F282-40CA-8DA0-39B43ED1A302}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{274CCE94-9ECE-40A4-87B8-1EFC0A5E9C77}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="main" sheetId="1" r:id="rId1"/>
     <sheet name="sozh" sheetId="2" r:id="rId2"/>
     <sheet name="detail_V_dis" sheetId="3" r:id="rId3"/>
+    <sheet name="detail_lambda" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -38,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="571" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="609" uniqueCount="21">
   <si>
     <t>exp</t>
   </si>
@@ -11886,7 +11887,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{19D26A40-5EC0-4FC2-A7B8-9E1205DD29FB}">
   <dimension ref="A1:H105"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A69" workbookViewId="0">
+    <sheetView topLeftCell="A69" workbookViewId="0">
       <selection activeCell="D105" sqref="D105"/>
     </sheetView>
   </sheetViews>
@@ -14625,4 +14626,597 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2364CF8B-C2BA-4C62-9862-215FAFAC0BAA}">
+  <dimension ref="A1:E34"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F27" sqref="F27"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2">
+        <v>1.8000000000000001E-4</v>
+      </c>
+      <c r="C2">
+        <v>160</v>
+      </c>
+      <c r="D2">
+        <v>0.2</v>
+      </c>
+      <c r="E2">
+        <v>0.99572192500000001</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3">
+        <v>2.0000000000000001E-4</v>
+      </c>
+      <c r="C3">
+        <v>160</v>
+      </c>
+      <c r="D3">
+        <v>0.2</v>
+      </c>
+      <c r="E3">
+        <v>0.99572192500000001</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4">
+        <v>2.5000000000000001E-4</v>
+      </c>
+      <c r="C4">
+        <v>160</v>
+      </c>
+      <c r="D4">
+        <v>0.2</v>
+      </c>
+      <c r="E4">
+        <v>0.99572192500000001</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5">
+        <v>2.9999999999999997E-4</v>
+      </c>
+      <c r="C5">
+        <v>160</v>
+      </c>
+      <c r="D5">
+        <v>0.2</v>
+      </c>
+      <c r="E5">
+        <v>0.996256684</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>3</v>
+      </c>
+      <c r="B6">
+        <v>3.5E-4</v>
+      </c>
+      <c r="C6">
+        <v>160</v>
+      </c>
+      <c r="D6">
+        <v>0.2</v>
+      </c>
+      <c r="E6">
+        <v>0.996256684</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>3</v>
+      </c>
+      <c r="B7">
+        <v>1.8000000000000001E-4</v>
+      </c>
+      <c r="C7">
+        <v>200</v>
+      </c>
+      <c r="D7">
+        <v>0.2</v>
+      </c>
+      <c r="E7">
+        <v>0.95080213899999999</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>3</v>
+      </c>
+      <c r="B8">
+        <v>2.0000000000000001E-4</v>
+      </c>
+      <c r="C8">
+        <v>200</v>
+      </c>
+      <c r="D8">
+        <v>0.2</v>
+      </c>
+      <c r="E8">
+        <v>0.98930481299999995</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>3</v>
+      </c>
+      <c r="B9">
+        <v>2.5000000000000001E-4</v>
+      </c>
+      <c r="C9">
+        <v>200</v>
+      </c>
+      <c r="D9">
+        <v>0.2</v>
+      </c>
+      <c r="E9">
+        <v>0.99358288800000005</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>3</v>
+      </c>
+      <c r="B10">
+        <v>2.9999999999999997E-4</v>
+      </c>
+      <c r="C10">
+        <v>200</v>
+      </c>
+      <c r="D10">
+        <v>0.2</v>
+      </c>
+      <c r="E10">
+        <v>0.99518716600000001</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>3</v>
+      </c>
+      <c r="B11">
+        <v>3.5E-4</v>
+      </c>
+      <c r="C11">
+        <v>200</v>
+      </c>
+      <c r="D11">
+        <v>0.2</v>
+      </c>
+      <c r="E11">
+        <v>0.99732620299999997</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>3</v>
+      </c>
+      <c r="B12">
+        <v>1.8000000000000001E-4</v>
+      </c>
+      <c r="C12">
+        <v>200</v>
+      </c>
+      <c r="D12">
+        <v>0.1</v>
+      </c>
+      <c r="E12">
+        <v>0.96243386200000003</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>3</v>
+      </c>
+      <c r="B13">
+        <v>1.8000000000000001E-4</v>
+      </c>
+      <c r="C13">
+        <v>240</v>
+      </c>
+      <c r="D13">
+        <v>0.2</v>
+      </c>
+      <c r="E13">
+        <v>0.74973261999999996</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>3</v>
+      </c>
+      <c r="B14">
+        <v>2.0000000000000001E-4</v>
+      </c>
+      <c r="C14">
+        <v>240</v>
+      </c>
+      <c r="D14">
+        <v>0.2</v>
+      </c>
+      <c r="E14">
+        <v>0.97433155100000002</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>3</v>
+      </c>
+      <c r="B15">
+        <v>2.5000000000000001E-4</v>
+      </c>
+      <c r="C15">
+        <v>240</v>
+      </c>
+      <c r="D15">
+        <v>0.2</v>
+      </c>
+      <c r="E15">
+        <v>0.98609625700000003</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>3</v>
+      </c>
+      <c r="B16">
+        <v>2.9999999999999997E-4</v>
+      </c>
+      <c r="C16">
+        <v>240</v>
+      </c>
+      <c r="D16">
+        <v>0.2</v>
+      </c>
+      <c r="E16">
+        <v>0.99144385000000002</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>3</v>
+      </c>
+      <c r="B17">
+        <v>3.5E-4</v>
+      </c>
+      <c r="C17">
+        <v>240</v>
+      </c>
+      <c r="D17">
+        <v>0.2</v>
+      </c>
+      <c r="E17">
+        <v>0.99518716600000001</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>3</v>
+      </c>
+      <c r="B18">
+        <v>1.8000000000000001E-4</v>
+      </c>
+      <c r="C18">
+        <v>240</v>
+      </c>
+      <c r="D18">
+        <v>0.05</v>
+      </c>
+      <c r="E18">
+        <v>0.93015873000000004</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>3</v>
+      </c>
+      <c r="B19">
+        <v>2.0000000000000001E-4</v>
+      </c>
+      <c r="C19">
+        <v>240</v>
+      </c>
+      <c r="D19">
+        <v>0.05</v>
+      </c>
+      <c r="E19">
+        <v>0.94973545000000004</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>3</v>
+      </c>
+      <c r="B20">
+        <v>2.5000000000000001E-4</v>
+      </c>
+      <c r="C20">
+        <v>240</v>
+      </c>
+      <c r="D20">
+        <v>0.05</v>
+      </c>
+      <c r="E20">
+        <v>0.97566137600000002</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>3</v>
+      </c>
+      <c r="B21">
+        <v>2.9999999999999997E-4</v>
+      </c>
+      <c r="C21">
+        <v>240</v>
+      </c>
+      <c r="D21">
+        <v>0.05</v>
+      </c>
+      <c r="E21">
+        <v>0.98783068799999996</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>3</v>
+      </c>
+      <c r="B22">
+        <v>3.5E-4</v>
+      </c>
+      <c r="C22">
+        <v>240</v>
+      </c>
+      <c r="D22">
+        <v>0.05</v>
+      </c>
+      <c r="E22">
+        <v>0.99523809500000004</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>3</v>
+      </c>
+      <c r="B23">
+        <v>1.8000000000000001E-4</v>
+      </c>
+      <c r="C23">
+        <v>240</v>
+      </c>
+      <c r="D23">
+        <v>0.1</v>
+      </c>
+      <c r="E23">
+        <v>0.92751322800000002</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>3</v>
+      </c>
+      <c r="B24">
+        <v>1.8000000000000001E-4</v>
+      </c>
+      <c r="C24">
+        <v>280</v>
+      </c>
+      <c r="D24">
+        <v>0.2</v>
+      </c>
+      <c r="E24">
+        <v>0.64973261999999998</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>3</v>
+      </c>
+      <c r="B25">
+        <v>2.0000000000000001E-4</v>
+      </c>
+      <c r="C25">
+        <v>280</v>
+      </c>
+      <c r="D25">
+        <v>0.2</v>
+      </c>
+      <c r="E25">
+        <v>0.91657754000000002</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>3</v>
+      </c>
+      <c r="B26">
+        <v>2.5000000000000001E-4</v>
+      </c>
+      <c r="C26">
+        <v>280</v>
+      </c>
+      <c r="D26">
+        <v>0.2</v>
+      </c>
+      <c r="E26">
+        <v>0.97754010700000005</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>3</v>
+      </c>
+      <c r="B27">
+        <v>2.9999999999999997E-4</v>
+      </c>
+      <c r="C27">
+        <v>280</v>
+      </c>
+      <c r="D27">
+        <v>0.2</v>
+      </c>
+      <c r="E27">
+        <v>0.98716577500000002</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>3</v>
+      </c>
+      <c r="B28">
+        <v>3.5E-4</v>
+      </c>
+      <c r="C28">
+        <v>280</v>
+      </c>
+      <c r="D28">
+        <v>0.2</v>
+      </c>
+      <c r="E28">
+        <v>0.99251336899999998</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>3</v>
+      </c>
+      <c r="B29">
+        <v>1.8000000000000001E-4</v>
+      </c>
+      <c r="C29">
+        <v>280</v>
+      </c>
+      <c r="D29">
+        <v>0.05</v>
+      </c>
+      <c r="E29">
+        <v>0.89470899500000001</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>3</v>
+      </c>
+      <c r="B30">
+        <v>2.0000000000000001E-4</v>
+      </c>
+      <c r="C30">
+        <v>280</v>
+      </c>
+      <c r="D30">
+        <v>0.05</v>
+      </c>
+      <c r="E30">
+        <v>0.91216931199999995</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>3</v>
+      </c>
+      <c r="B31">
+        <v>2.5000000000000001E-4</v>
+      </c>
+      <c r="C31">
+        <v>280</v>
+      </c>
+      <c r="D31">
+        <v>0.05</v>
+      </c>
+      <c r="E31">
+        <v>0.96137566100000005</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>3</v>
+      </c>
+      <c r="B32">
+        <v>2.9999999999999997E-4</v>
+      </c>
+      <c r="C32">
+        <v>280</v>
+      </c>
+      <c r="D32">
+        <v>0.05</v>
+      </c>
+      <c r="E32">
+        <v>0.98148148099999999</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>3</v>
+      </c>
+      <c r="B33">
+        <v>3.5E-4</v>
+      </c>
+      <c r="C33">
+        <v>280</v>
+      </c>
+      <c r="D33">
+        <v>0.05</v>
+      </c>
+      <c r="E33">
+        <v>0.98994709000000003</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>3</v>
+      </c>
+      <c r="B34">
+        <v>1.8000000000000001E-4</v>
+      </c>
+      <c r="C34">
+        <v>280</v>
+      </c>
+      <c r="D34">
+        <v>0.1</v>
+      </c>
+      <c r="E34">
+        <v>0.89894179900000004</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Ran part of the ye tests for validation of alpha
</commit_message>
<xml_diff>
--- a/Separator Model/Input/data_main.xlsx
+++ b/Separator Model/Input/data_main.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27932"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\iagr9\Projekte\MA\MA-Model_4\Separator Model\Input\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="T:\public\03 Studenten\00 Ausgeschieden\Ivan Guzman\05_Simulations\Abscheidermodell\MA\MA-Model_4\Separator Model\Input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D8DD418-0809-49B3-8D11-082D042A81F6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1EFBE033-F80E-442B-86A0-AABEE390BE6F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="main" sheetId="1" r:id="rId1"/>
@@ -33,6 +33,9 @@
         <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
         <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
+    </ext>
+    <ext xmlns:xlwcv="http://schemas.microsoft.com/office/spreadsheetml/2024/workbookCompatibilityVersion" uri="{D14903EA-33C4-47F7-8F05-3474C54BE107}">
+      <xlwcv:version setVersion="1"/>
     </ext>
   </extLst>
 </workbook>
@@ -194,7 +197,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Standard" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -474,11 +477,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:P110"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A91" workbookViewId="0">
-      <selection sqref="A1:I110"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="O6" sqref="O6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="7" max="7" width="7.5703125" bestFit="1" customWidth="1"/>
   </cols>
@@ -3689,7 +3692,7 @@
       <selection activeCell="M347" sqref="M347"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="3" max="3" width="12" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="18.42578125" bestFit="1" customWidth="1"/>
@@ -13146,7 +13149,7 @@
       <selection activeCell="D67" sqref="D67"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
@@ -15891,7 +15894,7 @@
       <selection activeCell="F27" sqref="F27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">

</xml_diff>

<commit_message>
Ran ye validation test final with determined alphas.
</commit_message>
<xml_diff>
--- a/Separator Model/Input/data_main.xlsx
+++ b/Separator Model/Input/data_main.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="T:\public\03 Studenten\00 Ausgeschieden\Ivan Guzman\05_Simulations\Abscheidermodell\MA\MA-Model_4\Separator Model\Input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1EFBE033-F80E-442B-86A0-AABEE390BE6F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A2C9036-8D1C-47EA-B6C9-4A1E58002713}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="main" sheetId="1" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="638" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="592" uniqueCount="23">
   <si>
     <t>exp</t>
   </si>
@@ -477,8 +477,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:P110"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O6" sqref="O6"/>
+    <sheetView topLeftCell="A69" workbookViewId="0">
+      <selection activeCell="A50" sqref="A50:D85"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -13143,15 +13143,15 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{19D26A40-5EC0-4FC2-A7B8-9E1205DD29FB}">
-  <dimension ref="A1:H105"/>
+  <dimension ref="A1:E63"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D67" sqref="D67"/>
+    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="E22" sqref="E22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -13164,2721 +13164,882 @@
       <c r="D1" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="E1" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="F1" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="G1" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="H1" s="4" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>14</v>
-      </c>
-      <c r="B2">
-        <v>2.0462099999999999E-4</v>
-      </c>
-      <c r="C2">
-        <v>743.10170100000005</v>
-      </c>
-      <c r="D2">
-        <v>0.29701893400000001</v>
-      </c>
-      <c r="E2">
-        <v>3.55819E-2</v>
-      </c>
-      <c r="F2">
-        <v>9.6633421999999997E-2</v>
-      </c>
-      <c r="G2">
-        <v>4.4652340000000002E-3</v>
-      </c>
-      <c r="H2">
-        <v>0.98750888400000003</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>14</v>
-      </c>
-      <c r="B3">
-        <v>6.5725699999999996E-4</v>
-      </c>
-      <c r="C3">
-        <v>748.36788460000002</v>
-      </c>
-      <c r="D3">
-        <v>0.50333939500000002</v>
-      </c>
-      <c r="E3">
-        <v>2.2846333E-2</v>
-      </c>
-      <c r="F3">
-        <v>9.2660582000000005E-2</v>
-      </c>
-      <c r="G3">
-        <v>1.528742E-3</v>
-      </c>
-      <c r="H3">
-        <v>0.99108918400000001</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>14</v>
-      </c>
-      <c r="B4">
-        <v>3.1127999999999999E-4</v>
-      </c>
-      <c r="C4">
-        <v>749.92972780000002</v>
-      </c>
-      <c r="D4">
-        <v>0.49988101000000001</v>
-      </c>
-      <c r="E4">
-        <v>3.3656999999999999E-2</v>
-      </c>
-      <c r="F4">
-        <v>0.10772396300000001</v>
-      </c>
-      <c r="G4">
-        <v>4.7552549999999999E-3</v>
-      </c>
-      <c r="H4">
-        <v>0.99268671900000005</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>14</v>
-      </c>
-      <c r="B5">
-        <v>4.4927699999999999E-4</v>
-      </c>
-      <c r="C5">
-        <v>749.97402599999998</v>
-      </c>
-      <c r="D5">
-        <v>0.399764919</v>
-      </c>
-      <c r="E5">
-        <v>3.2073999999999998E-2</v>
-      </c>
-      <c r="F5">
-        <v>9.5001253999999993E-2</v>
-      </c>
-      <c r="G5">
-        <v>3.785549E-3</v>
-      </c>
-      <c r="H5">
-        <v>0.98653263199999996</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>15</v>
-      </c>
-      <c r="B6">
-        <v>5.4967899999999997E-4</v>
-      </c>
-      <c r="C6">
-        <v>750.02556879999997</v>
-      </c>
-      <c r="D6">
-        <v>0.50015754999999995</v>
-      </c>
-      <c r="E6">
-        <v>3.8374125000000002E-2</v>
-      </c>
-      <c r="F6">
-        <v>0.101830843</v>
-      </c>
-      <c r="G6">
-        <v>5.2321299999999998E-3</v>
-      </c>
-      <c r="H6">
-        <v>0.99445781600000005</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>14</v>
-      </c>
-      <c r="B7">
-        <v>3.38769E-4</v>
-      </c>
-      <c r="C7">
-        <v>750.05733190000001</v>
-      </c>
-      <c r="D7">
-        <v>0.49989457599999998</v>
-      </c>
-      <c r="E7">
-        <v>3.2000428999999997E-2</v>
-      </c>
-      <c r="F7">
-        <v>0.108397884</v>
-      </c>
-      <c r="G7">
-        <v>4.1389720000000003E-3</v>
-      </c>
-      <c r="H7">
-        <v>0.99176721899999998</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>14</v>
-      </c>
-      <c r="B8">
-        <v>2.4194099999999999E-4</v>
-      </c>
-      <c r="C8">
-        <v>750.20782199999996</v>
-      </c>
-      <c r="D8">
-        <v>0.40002338700000001</v>
-      </c>
-      <c r="E8">
-        <v>2.9817666999999999E-2</v>
-      </c>
-      <c r="F8">
-        <v>0.106790285</v>
-      </c>
-      <c r="G8">
-        <v>5.2340670000000002E-3</v>
-      </c>
-      <c r="H8">
-        <v>0.99171526700000001</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>14</v>
-      </c>
-      <c r="B9">
-        <v>4.9274500000000005E-4</v>
-      </c>
-      <c r="C9">
-        <v>750.25178530000005</v>
-      </c>
-      <c r="D9">
-        <v>0.29988877800000002</v>
-      </c>
-      <c r="E9">
-        <v>2.9670385000000001E-2</v>
-      </c>
-      <c r="F9">
-        <v>0.10019613600000001</v>
-      </c>
-      <c r="G9">
-        <v>2.8000159999999998E-3</v>
-      </c>
-      <c r="H9">
-        <v>0.98938694400000005</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" s="1">
+        <v>2.5999999999999998E-4</v>
+      </c>
+      <c r="C2" s="1">
+        <v>160</v>
+      </c>
+      <c r="D2" s="1">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" s="1">
+        <v>2.81E-4</v>
+      </c>
+      <c r="C3" s="1">
+        <v>160</v>
+      </c>
+      <c r="D3" s="1">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" s="1">
+        <v>3.0699999999999998E-4</v>
+      </c>
+      <c r="C4" s="1">
+        <v>160</v>
+      </c>
+      <c r="D4" s="1">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" s="1">
+        <v>3.6999999999999999E-4</v>
+      </c>
+      <c r="C5" s="1">
+        <v>160</v>
+      </c>
+      <c r="D5" s="1">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B6" s="1">
+        <v>4.3100000000000001E-4</v>
+      </c>
+      <c r="C6" s="1">
+        <v>160</v>
+      </c>
+      <c r="D6" s="1">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B7" s="1">
+        <v>5.3200000000000003E-4</v>
+      </c>
+      <c r="C7" s="1">
+        <v>160</v>
+      </c>
+      <c r="D7" s="1">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B8" s="1">
+        <v>6.8900000000000005E-4</v>
+      </c>
+      <c r="C8" s="1">
+        <v>160</v>
+      </c>
+      <c r="D8" s="1">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B9" s="1">
+        <v>1.281E-3</v>
+      </c>
+      <c r="C9" s="1">
+        <v>160</v>
+      </c>
+      <c r="D9" s="1">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>16</v>
+        <v>3</v>
       </c>
       <c r="B10">
-        <v>6.1183099999999996E-4</v>
+        <v>2.52E-4</v>
       </c>
       <c r="C10">
-        <v>750.71744000000001</v>
+        <v>200</v>
       </c>
       <c r="D10">
-        <v>0.50033280999999996</v>
-      </c>
-      <c r="E10">
-        <v>2.9766384999999999E-2</v>
-      </c>
-      <c r="F10">
-        <v>9.8495864000000002E-2</v>
-      </c>
-      <c r="G10">
-        <v>3.1483090000000002E-3</v>
-      </c>
-      <c r="H10">
-        <v>0.99218971899999997</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>17</v>
+        <v>3</v>
       </c>
       <c r="B11">
-        <v>3.9097999999999997E-4</v>
+        <v>2.8299999999999999E-4</v>
       </c>
       <c r="C11">
-        <v>750.86723619999998</v>
+        <v>200</v>
       </c>
       <c r="D11">
-        <v>0.30092750000000001</v>
-      </c>
-      <c r="E11">
-        <v>3.4920187999999998E-2</v>
-      </c>
-      <c r="F11">
-        <v>0.100884113</v>
-      </c>
-      <c r="G11">
-        <v>3.2887580000000001E-3</v>
-      </c>
-      <c r="H11">
-        <v>0.99199386300000003</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>15</v>
+        <v>3</v>
       </c>
       <c r="B12">
-        <v>2.2167000000000001E-4</v>
+        <v>3.2499999999999999E-4</v>
       </c>
       <c r="C12">
-        <v>751.48936860000003</v>
+        <v>200</v>
       </c>
       <c r="D12">
-        <v>0.40003253100000002</v>
-      </c>
-      <c r="E12">
-        <v>1.9631529000000002E-2</v>
-      </c>
-      <c r="F12">
-        <v>0.11041532699999999</v>
-      </c>
-      <c r="G12">
-        <v>4.5576050000000002E-3</v>
-      </c>
-      <c r="H12">
-        <v>0.99505433700000001</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>15</v>
+        <v>3</v>
       </c>
       <c r="B13">
-        <v>6.7796600000000001E-4</v>
+        <v>3.8299999999999999E-4</v>
       </c>
       <c r="C13">
-        <v>752.85933369999998</v>
+        <v>200</v>
       </c>
       <c r="D13">
-        <v>0.49949943499999999</v>
-      </c>
-      <c r="E13">
-        <v>4.1055332999999999E-2</v>
-      </c>
-      <c r="F13">
-        <v>9.7580385000000006E-2</v>
-      </c>
-      <c r="G13">
-        <v>3.6210349999999999E-3</v>
-      </c>
-      <c r="H13">
-        <v>0.99436792399999996</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>17</v>
+        <v>3</v>
       </c>
       <c r="B14">
-        <v>2.54348E-4</v>
+        <v>4.64E-4</v>
       </c>
       <c r="C14">
-        <v>908.35374130000002</v>
+        <v>200</v>
       </c>
       <c r="D14">
-        <v>0.27718706700000001</v>
-      </c>
-      <c r="E14">
-        <v>1.9585846000000001E-2</v>
-      </c>
-      <c r="F14">
-        <v>0.103970942</v>
-      </c>
-      <c r="G14">
-        <v>3.6805710000000001E-3</v>
-      </c>
-      <c r="H14">
-        <v>0.99263151500000002</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>11</v>
+        <v>3</v>
       </c>
       <c r="B15">
-        <v>8.0239500000000002E-4</v>
+        <v>5.8399999999999999E-4</v>
       </c>
       <c r="C15">
-        <v>998.44373169999994</v>
+        <v>200</v>
       </c>
       <c r="D15">
-        <v>0.499859416</v>
-      </c>
-      <c r="E15">
-        <v>1.5360333E-2</v>
-      </c>
-      <c r="F15">
-        <v>0.10280117799999999</v>
-      </c>
-      <c r="G15">
-        <v>3.8602500000000002E-4</v>
-      </c>
-      <c r="H15">
-        <v>0.99546705300000005</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>16</v>
+        <v>3</v>
       </c>
       <c r="B16">
-        <v>5.0275999999999999E-4</v>
+        <v>7.8799999999999996E-4</v>
       </c>
       <c r="C16">
-        <v>999.40820970000004</v>
+        <v>200</v>
       </c>
       <c r="D16">
-        <v>0.29920427599999999</v>
-      </c>
-      <c r="E16">
-        <v>3.5955842000000002E-2</v>
-      </c>
-      <c r="F16">
-        <v>0.101860464</v>
-      </c>
-      <c r="G16">
-        <v>4.1493759999999998E-3</v>
-      </c>
-      <c r="H16">
-        <v>0.98989876499999996</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>11</v>
+        <v>3</v>
       </c>
       <c r="B17">
-        <v>5.9944000000000002E-4</v>
+        <v>1.0950000000000001E-3</v>
       </c>
       <c r="C17">
-        <v>999.59662909999997</v>
+        <v>200</v>
       </c>
       <c r="D17">
-        <v>0.40006547100000001</v>
-      </c>
-      <c r="E17">
-        <v>0</v>
-      </c>
-      <c r="F17">
-        <v>9.7689174000000004E-2</v>
-      </c>
-      <c r="G17">
-        <v>4.8635799999999999E-4</v>
-      </c>
-      <c r="H17">
-        <v>0.99499302099999998</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>13</v>
+        <v>3</v>
       </c>
       <c r="B18">
-        <v>7.1244500000000003E-4</v>
+        <v>1.5E-3</v>
       </c>
       <c r="C18">
-        <v>999.64467930000001</v>
+        <v>200</v>
       </c>
       <c r="D18">
-        <v>0.49991358299999999</v>
-      </c>
-      <c r="E18">
-        <v>1.5761217000000001E-2</v>
-      </c>
-      <c r="F18">
-        <v>9.4884389999999999E-2</v>
-      </c>
-      <c r="G18">
-        <v>2.2179650000000001E-3</v>
-      </c>
-      <c r="H18">
-        <v>0.99704778699999996</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>14</v>
-      </c>
-      <c r="B19">
-        <v>3.7785800000000001E-4</v>
-      </c>
-      <c r="C19">
-        <v>999.67359969999995</v>
-      </c>
-      <c r="D19">
-        <v>0.30006925000000001</v>
-      </c>
-      <c r="E19">
-        <v>2.6276999999999998E-2</v>
-      </c>
-      <c r="F19">
-        <v>0.108183192</v>
-      </c>
-      <c r="G19">
-        <v>4.052745E-3</v>
-      </c>
-      <c r="H19">
-        <v>0.98579144299999999</v>
-      </c>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>13</v>
-      </c>
-      <c r="B20">
-        <v>5.6844399999999998E-4</v>
-      </c>
-      <c r="C20">
-        <v>1000.032227</v>
-      </c>
-      <c r="D20">
-        <v>0.29996158899999997</v>
-      </c>
-      <c r="E20">
-        <v>1.6771635999999999E-2</v>
-      </c>
-      <c r="F20">
-        <v>9.7314092000000005E-2</v>
-      </c>
-      <c r="G20">
-        <v>2.175696E-3</v>
-      </c>
-      <c r="H20">
-        <v>0.995888047</v>
-      </c>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
-        <v>17</v>
-      </c>
-      <c r="B21">
-        <v>6.5962200000000001E-4</v>
-      </c>
-      <c r="C21">
-        <v>1000.129858</v>
-      </c>
-      <c r="D21">
-        <v>0.49965211700000001</v>
-      </c>
-      <c r="E21">
-        <v>3.9373499999999999E-2</v>
-      </c>
-      <c r="F21">
-        <v>0.10375522299999999</v>
-      </c>
-      <c r="G21">
-        <v>5.4323920000000003E-3</v>
-      </c>
-      <c r="H21">
-        <v>0.99410157700000001</v>
-      </c>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
-        <v>13</v>
-      </c>
-      <c r="B22">
-        <v>7.5361500000000001E-4</v>
-      </c>
-      <c r="C22">
-        <v>1000.183129</v>
-      </c>
-      <c r="D22">
-        <v>0.50001522700000001</v>
-      </c>
-      <c r="E22">
-        <v>1.5923438000000002E-2</v>
-      </c>
-      <c r="F22">
-        <v>9.5239508E-2</v>
-      </c>
-      <c r="G22">
-        <v>2.0156449999999999E-3</v>
-      </c>
-      <c r="H22">
-        <v>0.99718886500000004</v>
-      </c>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
-        <v>15</v>
-      </c>
-      <c r="B23">
-        <v>3.65507E-4</v>
-      </c>
-      <c r="C23">
-        <v>1000.201091</v>
-      </c>
-      <c r="D23">
-        <v>0.30000356700000003</v>
-      </c>
-      <c r="E23">
-        <v>2.9010142999999999E-2</v>
-      </c>
-      <c r="F23">
-        <v>0.114449734</v>
-      </c>
-      <c r="G23">
-        <v>4.440495E-3</v>
-      </c>
-      <c r="H23">
-        <v>0.99139601200000005</v>
-      </c>
-    </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
-        <v>17</v>
-      </c>
-      <c r="B24">
-        <v>3.21902E-4</v>
-      </c>
-      <c r="C24">
-        <v>1000.303949</v>
-      </c>
-      <c r="D24">
-        <v>0.50013415000000006</v>
-      </c>
-      <c r="E24">
-        <v>2.9240461999999998E-2</v>
-      </c>
-      <c r="F24">
-        <v>0.11521322000000001</v>
-      </c>
-      <c r="G24">
-        <v>4.8777610000000004E-3</v>
-      </c>
-      <c r="H24">
-        <v>0.99550441999999995</v>
-      </c>
-    </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
-        <v>16</v>
-      </c>
-      <c r="B25">
-        <v>4.4690600000000001E-4</v>
-      </c>
-      <c r="C25">
-        <v>1000.564352</v>
-      </c>
-      <c r="D25">
-        <v>0.40118413600000002</v>
-      </c>
-      <c r="E25">
-        <v>3.6132938000000003E-2</v>
-      </c>
-      <c r="F25">
-        <v>0.10055367599999999</v>
-      </c>
-      <c r="G25">
-        <v>4.5400780000000003E-3</v>
-      </c>
-      <c r="H25">
-        <v>0.98875126400000002</v>
-      </c>
-    </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
-        <v>17</v>
-      </c>
-      <c r="B26">
-        <v>2.6539199999999998E-4</v>
-      </c>
-      <c r="C26">
-        <v>1002.961609</v>
-      </c>
-      <c r="D26">
-        <v>0.30087852900000001</v>
-      </c>
-      <c r="E26">
-        <v>2.4022870000000002E-2</v>
-      </c>
-      <c r="F26">
-        <v>0.10911349100000001</v>
-      </c>
-      <c r="G26">
-        <v>5.1225200000000002E-3</v>
-      </c>
-      <c r="H26">
-        <v>0.99228384400000003</v>
-      </c>
-    </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
-        <v>15</v>
-      </c>
-      <c r="B27">
-        <v>2.7240599999999999E-4</v>
-      </c>
-      <c r="C27">
-        <v>1242.8563799999999</v>
-      </c>
-      <c r="D27">
-        <v>0.29883443599999998</v>
-      </c>
-      <c r="E27">
-        <v>2.9332111000000001E-2</v>
-      </c>
-      <c r="F27">
-        <v>0.11349644</v>
-      </c>
-      <c r="G27">
-        <v>5.5628220000000003E-3</v>
-      </c>
-      <c r="H27">
-        <v>0.99175836900000003</v>
-      </c>
-    </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B19" s="1">
+        <v>2.7099999999999997E-4</v>
+      </c>
+      <c r="C19" s="1">
+        <v>240</v>
+      </c>
+      <c r="D19" s="1">
+        <v>0.2</v>
+      </c>
+      <c r="E19" s="1"/>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B20" s="1">
+        <v>2.9799999999999998E-4</v>
+      </c>
+      <c r="C20" s="1">
+        <v>240</v>
+      </c>
+      <c r="D20" s="1">
+        <v>0.2</v>
+      </c>
+      <c r="E20" s="1"/>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A21" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B21" s="1">
+        <v>3.4299999999999999E-4</v>
+      </c>
+      <c r="C21" s="1">
+        <v>240</v>
+      </c>
+      <c r="D21" s="1">
+        <v>0.2</v>
+      </c>
+      <c r="E21" s="1"/>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A22" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B22" s="1">
+        <v>4.0400000000000001E-4</v>
+      </c>
+      <c r="C22" s="1">
+        <v>240</v>
+      </c>
+      <c r="D22" s="1">
+        <v>0.2</v>
+      </c>
+      <c r="E22" s="1"/>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A23" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B23" s="1">
+        <v>5.0299999999999997E-4</v>
+      </c>
+      <c r="C23" s="1">
+        <v>240</v>
+      </c>
+      <c r="D23" s="1">
+        <v>0.2</v>
+      </c>
+      <c r="E23" s="1"/>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A24" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B24" s="1">
+        <v>6.0999999999999997E-4</v>
+      </c>
+      <c r="C24" s="1">
+        <v>240</v>
+      </c>
+      <c r="D24" s="1">
+        <v>0.2</v>
+      </c>
+      <c r="E24" s="1"/>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A25" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B25" s="1">
+        <v>8.0400000000000003E-4</v>
+      </c>
+      <c r="C25" s="1">
+        <v>240</v>
+      </c>
+      <c r="D25" s="1">
+        <v>0.2</v>
+      </c>
+      <c r="E25" s="1"/>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A26" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B26" s="1">
+        <v>1.0920000000000001E-3</v>
+      </c>
+      <c r="C26" s="1">
+        <v>240</v>
+      </c>
+      <c r="D26" s="1">
+        <v>0.2</v>
+      </c>
+      <c r="E26" s="1"/>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A27" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B27" s="1">
+        <v>1.4159999999999999E-3</v>
+      </c>
+      <c r="C27" s="1">
+        <v>240</v>
+      </c>
+      <c r="D27" s="1">
+        <v>0.2</v>
+      </c>
+      <c r="E27" s="1"/>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>15</v>
+        <v>3</v>
       </c>
       <c r="B28">
-        <v>5.6636299999999996E-4</v>
+        <v>2.5399999999999999E-4</v>
       </c>
       <c r="C28">
-        <v>1249.038305</v>
+        <v>280</v>
       </c>
       <c r="D28">
-        <v>0.50009379399999998</v>
-      </c>
-      <c r="E28">
-        <v>3.3174416999999998E-2</v>
-      </c>
-      <c r="F28">
-        <v>0.114298685</v>
-      </c>
-      <c r="G28">
-        <v>5.8367810000000001E-3</v>
-      </c>
-      <c r="H28">
-        <v>0.99043759600000003</v>
-      </c>
-    </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>15</v>
+        <v>3</v>
       </c>
       <c r="B29">
-        <v>4.4455299999999998E-4</v>
+        <v>2.9399999999999999E-4</v>
       </c>
       <c r="C29">
-        <v>1249.8621929999999</v>
+        <v>280</v>
       </c>
       <c r="D29">
-        <v>0.29980042600000001</v>
-      </c>
-      <c r="E29">
-        <v>2.8255058999999999E-2</v>
-      </c>
-      <c r="F29">
-        <v>0.10856081200000001</v>
-      </c>
-      <c r="G29">
-        <v>3.8722560000000001E-3</v>
-      </c>
-      <c r="H29">
-        <v>0.98956896599999999</v>
-      </c>
-    </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>14</v>
+        <v>3</v>
       </c>
       <c r="B30">
-        <v>3.4781999999999999E-4</v>
+        <v>3.3700000000000001E-4</v>
       </c>
       <c r="C30">
-        <v>1249.9720520000001</v>
+        <v>280</v>
       </c>
       <c r="D30">
-        <v>0.29999618500000003</v>
-      </c>
-      <c r="E30">
-        <v>4.2983100000000003E-2</v>
-      </c>
-      <c r="F30">
-        <v>0.10975439100000001</v>
-      </c>
-      <c r="G30">
-        <v>4.7517119999999999E-3</v>
-      </c>
-      <c r="H30">
-        <v>0.98241363800000003</v>
-      </c>
-    </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>16</v>
+        <v>3</v>
       </c>
       <c r="B31">
-        <v>3.0862499999999998E-4</v>
+        <v>4.0200000000000001E-4</v>
       </c>
       <c r="C31">
-        <v>1250.009063</v>
+        <v>280</v>
       </c>
       <c r="D31">
-        <v>0.300016848</v>
-      </c>
-      <c r="E31">
-        <v>3.03678E-2</v>
-      </c>
-      <c r="F31">
-        <v>0.107568497</v>
-      </c>
-      <c r="G31">
-        <v>4.6496790000000003E-3</v>
-      </c>
-      <c r="H31">
-        <v>0.98361751799999997</v>
-      </c>
-    </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>17</v>
+        <v>3</v>
       </c>
       <c r="B32">
-        <v>3.9580799999999999E-4</v>
+        <v>4.9700000000000005E-4</v>
       </c>
       <c r="C32">
-        <v>1250.0364039999999</v>
+        <v>280</v>
       </c>
       <c r="D32">
-        <v>0.29999587</v>
-      </c>
-      <c r="E32">
-        <v>2.3775000000000001E-2</v>
-      </c>
-      <c r="F32">
-        <v>0.11548971800000001</v>
-      </c>
-      <c r="G32">
-        <v>4.2850120000000004E-3</v>
-      </c>
-      <c r="H32">
-        <v>0.99005631800000005</v>
-      </c>
-    </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>17</v>
+        <v>3</v>
       </c>
       <c r="B33">
-        <v>4.85129E-4</v>
+        <v>6.1700000000000004E-4</v>
       </c>
       <c r="C33">
-        <v>1250.056002</v>
+        <v>280</v>
       </c>
       <c r="D33">
-        <v>0.30007985999999998</v>
-      </c>
-      <c r="E33">
-        <v>2.7580614999999999E-2</v>
-      </c>
-      <c r="F33">
-        <v>0.11381099</v>
-      </c>
-      <c r="G33">
-        <v>4.0394979999999999E-3</v>
-      </c>
-      <c r="H33">
-        <v>0.99273382399999999</v>
-      </c>
-    </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>17</v>
+        <v>3</v>
       </c>
       <c r="B34">
-        <v>4.7428800000000001E-4</v>
+        <v>8.0000000000000004E-4</v>
       </c>
       <c r="C34">
-        <v>1250.0886849999999</v>
+        <v>280</v>
       </c>
       <c r="D34">
-        <v>0.30001281800000001</v>
-      </c>
-      <c r="E34">
-        <v>2.8364166999999999E-2</v>
-      </c>
-      <c r="F34">
-        <v>0.11308117199999999</v>
-      </c>
-      <c r="G34">
-        <v>5.2047889999999996E-3</v>
-      </c>
-      <c r="H34">
-        <v>0.99108814999999995</v>
-      </c>
-    </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>15</v>
+        <v>3</v>
       </c>
       <c r="B35">
-        <v>3.4672300000000001E-4</v>
+        <v>1.0989999999999999E-3</v>
       </c>
       <c r="C35">
-        <v>1250.9434040000001</v>
+        <v>280</v>
       </c>
       <c r="D35">
-        <v>0.39999618199999998</v>
-      </c>
-      <c r="E35">
-        <v>3.9580443999999999E-2</v>
-      </c>
-      <c r="F35">
-        <v>0.110695898</v>
-      </c>
-      <c r="G35">
-        <v>6.4767380000000001E-3</v>
-      </c>
-      <c r="H35">
-        <v>0.99251876100000003</v>
-      </c>
-    </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>14</v>
+        <v>3</v>
       </c>
       <c r="B36">
-        <v>5.7827599999999996E-4</v>
+        <v>1.2780000000000001E-3</v>
       </c>
       <c r="C36">
-        <v>1252.670832</v>
+        <v>280</v>
       </c>
       <c r="D36">
-        <v>0.49995556099999999</v>
-      </c>
-      <c r="E36">
-        <v>4.6688437999999999E-2</v>
-      </c>
-      <c r="F36">
-        <v>9.5985962999999994E-2</v>
-      </c>
-      <c r="G36">
-        <v>5.6972220000000001E-3</v>
-      </c>
-      <c r="H36">
-        <v>0.98525604600000005</v>
-      </c>
-    </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>16</v>
+        <v>3</v>
       </c>
       <c r="B37">
-        <v>4.6433100000000001E-4</v>
+        <v>2.2510799999999999E-4</v>
       </c>
       <c r="C37">
-        <v>1255.424561</v>
+        <v>280</v>
       </c>
       <c r="D37">
-        <v>0.39989443400000002</v>
-      </c>
-      <c r="E37">
-        <v>3.2895832999999999E-2</v>
-      </c>
-      <c r="F37">
-        <v>0.10475915299999999</v>
-      </c>
-      <c r="G37">
-        <v>4.4100290000000002E-3</v>
-      </c>
-      <c r="H37">
-        <v>0.98489914300000003</v>
-      </c>
-    </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>15</v>
+        <v>3</v>
       </c>
       <c r="B38">
-        <v>4.11395E-4</v>
+        <v>2.5108200000000002E-4</v>
       </c>
       <c r="C38">
-        <v>1267.5140690000001</v>
+        <v>280</v>
       </c>
       <c r="D38">
-        <v>0.49920661399999999</v>
-      </c>
-      <c r="E38">
-        <v>2.7389750000000001E-2</v>
-      </c>
-      <c r="F38">
-        <v>0.12562072899999999</v>
-      </c>
-      <c r="G38">
-        <v>3.9256580000000003E-3</v>
-      </c>
-      <c r="H38">
-        <v>0.99312282299999999</v>
-      </c>
-    </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>15</v>
+        <v>3</v>
       </c>
       <c r="B39">
-        <v>3.13467E-4</v>
+        <v>2.8571400000000001E-4</v>
       </c>
       <c r="C39">
-        <v>1271.3936630000001</v>
+        <v>280</v>
       </c>
       <c r="D39">
-        <v>0.40056073800000003</v>
-      </c>
-      <c r="E39">
-        <v>3.3499599999999997E-2</v>
-      </c>
-      <c r="F39">
-        <v>0.11312243299999999</v>
-      </c>
-      <c r="G39">
-        <v>5.9295399999999996E-3</v>
-      </c>
-      <c r="H39">
-        <v>0.99374623100000004</v>
-      </c>
-    </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>13</v>
+        <v>3</v>
       </c>
       <c r="B40">
-        <v>7.2654800000000004E-4</v>
+        <v>3.3419899999999998E-4</v>
       </c>
       <c r="C40">
-        <v>1455.6305829999999</v>
+        <v>280</v>
       </c>
       <c r="D40">
-        <v>0.49692148400000002</v>
-      </c>
-      <c r="E40">
-        <v>1.6203833000000001E-2</v>
-      </c>
-      <c r="F40">
-        <v>9.1711663999999998E-2</v>
-      </c>
-      <c r="G40">
-        <v>2.966729E-3</v>
-      </c>
-      <c r="H40">
-        <v>0.99718670099999995</v>
-      </c>
-    </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>13</v>
+        <v>3</v>
       </c>
       <c r="B41">
-        <v>8.1662800000000002E-4</v>
+        <v>4.0000000000000002E-4</v>
       </c>
       <c r="C41">
-        <v>1492.737848</v>
+        <v>280</v>
       </c>
       <c r="D41">
-        <v>0.50025813699999999</v>
-      </c>
-      <c r="E41">
-        <v>2.5555333E-2</v>
-      </c>
-      <c r="F41">
-        <v>9.2475197999999995E-2</v>
-      </c>
-      <c r="G41">
-        <v>2.9827109999999999E-3</v>
-      </c>
-      <c r="H41">
-        <v>0.99533773199999998</v>
-      </c>
-    </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>13</v>
+        <v>3</v>
       </c>
       <c r="B42">
-        <v>8.5975099999999996E-4</v>
+        <v>5.0216499999999995E-4</v>
       </c>
       <c r="C42">
-        <v>1494.673636</v>
+        <v>280</v>
       </c>
       <c r="D42">
-        <v>0.50000099099999995</v>
-      </c>
-      <c r="E42">
-        <v>2.7710216999999999E-2</v>
-      </c>
-      <c r="F42">
-        <v>9.1934420000000003E-2</v>
-      </c>
-      <c r="G42">
-        <v>2.846627E-3</v>
-      </c>
-      <c r="H42">
-        <v>0.99697522500000002</v>
-      </c>
-    </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>12</v>
+        <v>3</v>
       </c>
       <c r="B43">
-        <v>7.0617800000000001E-4</v>
+        <v>6.44156E-4</v>
       </c>
       <c r="C43">
-        <v>1497.1705119999999</v>
+        <v>280</v>
       </c>
       <c r="D43">
-        <v>0.49990232400000001</v>
-      </c>
-      <c r="E43">
-        <v>1.9429286E-2</v>
-      </c>
-      <c r="F43">
-        <v>9.1588153000000005E-2</v>
-      </c>
-      <c r="G43">
-        <v>3.0430520000000001E-3</v>
-      </c>
-      <c r="H43">
-        <v>0.99707969600000002</v>
-      </c>
-    </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>11</v>
+        <v>3</v>
       </c>
       <c r="B44">
-        <v>6.3737199999999998E-4</v>
+        <v>9.904759999999999E-4</v>
       </c>
       <c r="C44">
-        <v>1500.051467</v>
+        <v>280</v>
       </c>
       <c r="D44">
-        <v>0.29994249899999997</v>
-      </c>
-      <c r="E44">
-        <v>2.6298999999999999E-2</v>
-      </c>
-      <c r="F44">
-        <v>0.10857765</v>
-      </c>
-      <c r="G44">
-        <v>7.1048200000000002E-4</v>
-      </c>
-      <c r="H44">
-        <v>0.99349073799999998</v>
-      </c>
-    </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>13</v>
+        <v>3</v>
       </c>
       <c r="B45">
-        <v>5.2616900000000005E-4</v>
+        <v>1.4112549999999999E-3</v>
       </c>
       <c r="C45">
-        <v>1500.0874120000001</v>
+        <v>280</v>
       </c>
       <c r="D45">
-        <v>0.30007125099999998</v>
-      </c>
-      <c r="E45">
-        <v>1.9176444000000001E-2</v>
-      </c>
-      <c r="F45">
-        <v>0.12915310899999999</v>
-      </c>
-      <c r="G45">
-        <v>7.8471699999999999E-4</v>
-      </c>
-      <c r="H45">
-        <v>0.99525415699999997</v>
-      </c>
-    </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>11</v>
+        <v>3</v>
       </c>
       <c r="B46">
-        <v>7.4180700000000003E-4</v>
+        <v>2.4242400000000001E-4</v>
       </c>
       <c r="C46">
-        <v>1500.215265</v>
+        <v>280</v>
       </c>
       <c r="D46">
-        <v>0.39993976599999997</v>
-      </c>
-      <c r="E46">
-        <v>4.5705333000000001E-2</v>
-      </c>
-      <c r="F46">
-        <v>9.7766817000000006E-2</v>
-      </c>
-      <c r="G46">
-        <v>4.3964299999999998E-4</v>
-      </c>
-      <c r="H46">
-        <v>0.99480906899999999</v>
-      </c>
-    </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>11</v>
+        <v>3</v>
       </c>
       <c r="B47">
-        <v>9.1292700000000001E-4</v>
+        <v>2.7186099999999998E-4</v>
       </c>
       <c r="C47">
-        <v>1500.5413000000001</v>
+        <v>280</v>
       </c>
       <c r="D47">
-        <v>0.50044513199999996</v>
-      </c>
-      <c r="E47">
-        <v>2.2795666999999999E-2</v>
-      </c>
-      <c r="F47">
-        <v>0.103834646</v>
-      </c>
-      <c r="G47">
-        <v>4.4096199999999998E-4</v>
-      </c>
-      <c r="H47">
-        <v>0.99445706499999997</v>
-      </c>
-    </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A48" t="s">
-        <v>11</v>
-      </c>
-      <c r="B48">
-        <v>9.4360899999999998E-4</v>
-      </c>
-      <c r="C48">
-        <v>1500.993866</v>
-      </c>
-      <c r="D48">
-        <v>0.499986655</v>
-      </c>
-      <c r="E48">
-        <v>2.3137000000000001E-2</v>
-      </c>
-      <c r="F48">
-        <v>0.103615651</v>
-      </c>
-      <c r="G48">
-        <v>8.3131500000000001E-4</v>
-      </c>
-      <c r="H48">
-        <v>0.99464200000000003</v>
-      </c>
-    </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A49" t="s">
-        <v>13</v>
-      </c>
-      <c r="B49">
-        <v>6.1466400000000001E-4</v>
-      </c>
-      <c r="C49">
-        <v>1502.4972680000001</v>
-      </c>
-      <c r="D49">
-        <v>0.40017336999999997</v>
-      </c>
-      <c r="E49">
-        <v>1.6598000000000002E-2</v>
-      </c>
-      <c r="F49">
-        <v>9.4777095000000006E-2</v>
-      </c>
-      <c r="G49">
-        <v>2.47956E-3</v>
-      </c>
-      <c r="H49">
-        <v>0.99691817900000002</v>
-      </c>
-    </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A50" t="s">
-        <v>13</v>
-      </c>
-      <c r="B50">
-        <v>6.6162899999999995E-4</v>
-      </c>
-      <c r="C50">
-        <v>1504.5464079999999</v>
-      </c>
-      <c r="D50">
-        <v>0.40074769799999999</v>
-      </c>
-      <c r="E50">
-        <v>1.9850666999999999E-2</v>
-      </c>
-      <c r="F50">
-        <v>9.4852504000000004E-2</v>
-      </c>
-      <c r="G50">
-        <v>2.9607710000000001E-3</v>
-      </c>
-      <c r="H50">
-        <v>0.99641502000000004</v>
-      </c>
-    </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A51" t="s">
-        <v>13</v>
-      </c>
-      <c r="B51">
-        <v>7.2370699999999997E-4</v>
-      </c>
-      <c r="C51">
-        <v>1752.5926159999999</v>
-      </c>
-      <c r="D51">
-        <v>0.50002069100000002</v>
-      </c>
-      <c r="E51">
-        <v>2.4327778000000001E-2</v>
-      </c>
-      <c r="F51">
-        <v>9.0262732999999998E-2</v>
-      </c>
-      <c r="G51">
-        <v>2.7651020000000002E-3</v>
-      </c>
-      <c r="H51">
-        <v>0.99688110399999996</v>
-      </c>
-    </row>
-    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A52" t="s">
-        <v>11</v>
-      </c>
-      <c r="B52">
-        <v>8.0128199999999995E-4</v>
-      </c>
-      <c r="C52">
-        <v>1995.9935250000001</v>
-      </c>
-      <c r="D52">
-        <v>0.49970003499999999</v>
-      </c>
-      <c r="E52">
-        <v>2.9573833000000001E-2</v>
-      </c>
-      <c r="F52">
-        <v>0.101849986</v>
-      </c>
-      <c r="G52">
-        <v>6.1271999999999997E-4</v>
-      </c>
-      <c r="H52">
-        <v>0.99330616800000004</v>
-      </c>
-    </row>
-    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A53" t="s">
-        <v>13</v>
-      </c>
-      <c r="B53">
-        <v>6.8117199999999996E-4</v>
-      </c>
-      <c r="C53">
-        <v>1999.6194820000001</v>
-      </c>
-      <c r="D53">
-        <v>0.49998881699999997</v>
-      </c>
-      <c r="E53">
-        <v>2.3282932999999999E-2</v>
-      </c>
-      <c r="F53">
-        <v>8.8787929000000002E-2</v>
-      </c>
-      <c r="G53">
-        <v>2.7722139999999998E-3</v>
-      </c>
-      <c r="H53">
-        <v>0.99639685600000005</v>
-      </c>
-    </row>
-    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A54" t="s">
-        <v>13</v>
-      </c>
-      <c r="B54">
-        <v>6.1575900000000001E-4</v>
-      </c>
-      <c r="C54">
-        <v>1999.9767119999999</v>
-      </c>
-      <c r="D54">
-        <v>0.40001579300000001</v>
-      </c>
-      <c r="E54">
-        <v>3.4569500000000003E-2</v>
-      </c>
-      <c r="F54">
-        <v>9.3052383000000002E-2</v>
-      </c>
-      <c r="G54">
-        <v>1.4778720000000001E-3</v>
-      </c>
-      <c r="H54">
-        <v>0.99505876199999999</v>
-      </c>
-    </row>
-    <row r="55" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A55" t="s">
-        <v>13</v>
-      </c>
-      <c r="B55">
-        <v>5.7284199999999995E-4</v>
-      </c>
-      <c r="C55">
-        <v>2000.4061589999999</v>
-      </c>
-      <c r="D55">
-        <v>0.40002267499999999</v>
-      </c>
-      <c r="E55">
-        <v>2.1106E-2</v>
-      </c>
-      <c r="F55">
-        <v>8.9342075000000007E-2</v>
-      </c>
-      <c r="G55">
-        <v>1.5362749999999999E-3</v>
-      </c>
-      <c r="H55">
-        <v>0.99545406299999994</v>
-      </c>
-    </row>
-    <row r="56" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A56" t="s">
-        <v>12</v>
-      </c>
-      <c r="B56">
-        <v>7.3430900000000005E-4</v>
-      </c>
-      <c r="C56">
-        <v>2000.6603399999999</v>
-      </c>
-      <c r="D56">
-        <v>0.50012684799999996</v>
-      </c>
-      <c r="E56">
-        <v>2.0743889000000001E-2</v>
-      </c>
-      <c r="F56">
-        <v>8.9674559000000001E-2</v>
-      </c>
-      <c r="G56">
-        <v>3.0504239999999999E-3</v>
-      </c>
-      <c r="H56">
-        <v>0.99543250999999999</v>
-      </c>
-    </row>
-    <row r="57" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A57" t="s">
-        <v>3</v>
-      </c>
-      <c r="B57">
-        <v>2.5999999999999998E-4</v>
-      </c>
-      <c r="C57">
-        <v>160</v>
-      </c>
-      <c r="D57">
-        <v>0.2</v>
-      </c>
-      <c r="E57">
-        <v>0</v>
-      </c>
-      <c r="F57">
-        <v>0</v>
-      </c>
-      <c r="G57">
-        <v>9.6295699999999996E-4</v>
-      </c>
-      <c r="H57">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="58" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A58" t="s">
-        <v>3</v>
-      </c>
-      <c r="B58">
-        <v>2.81E-4</v>
-      </c>
-      <c r="C58">
-        <v>160</v>
-      </c>
-      <c r="D58">
-        <v>0.2</v>
-      </c>
-      <c r="E58">
-        <v>0</v>
-      </c>
-      <c r="F58">
-        <v>0</v>
-      </c>
-      <c r="G58">
-        <v>5.4068499999999995E-4</v>
-      </c>
-      <c r="H58">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="59" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A59" t="s">
-        <v>3</v>
-      </c>
-      <c r="B59">
-        <v>3.0699999999999998E-4</v>
-      </c>
-      <c r="C59">
-        <v>160</v>
-      </c>
-      <c r="D59">
-        <v>0.2</v>
-      </c>
-      <c r="E59">
-        <v>0</v>
-      </c>
-      <c r="F59">
-        <v>0</v>
-      </c>
-      <c r="G59">
-        <v>5.7356200000000001E-4</v>
-      </c>
-      <c r="H59">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="60" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A60" t="s">
-        <v>3</v>
-      </c>
-      <c r="B60">
-        <v>3.6999999999999999E-4</v>
-      </c>
-      <c r="C60">
-        <v>160</v>
-      </c>
-      <c r="D60">
-        <v>0.2</v>
-      </c>
-      <c r="E60">
-        <v>0</v>
-      </c>
-      <c r="F60">
-        <v>0</v>
-      </c>
-      <c r="G60">
-        <v>1.609114E-3</v>
-      </c>
-      <c r="H60">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="61" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A61" t="s">
-        <v>3</v>
-      </c>
-      <c r="B61">
-        <v>4.3100000000000001E-4</v>
-      </c>
-      <c r="C61">
-        <v>160</v>
-      </c>
-      <c r="D61">
-        <v>0.2</v>
-      </c>
-      <c r="E61">
-        <v>0</v>
-      </c>
-      <c r="F61">
-        <v>0</v>
-      </c>
-      <c r="G61">
-        <v>2.0221039999999998E-3</v>
-      </c>
-      <c r="H61">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="62" spans="1:8" x14ac:dyDescent="0.25">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A48" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B48" s="1">
+        <v>3.0995699999999997E-4</v>
+      </c>
+      <c r="C48" s="1">
+        <v>280</v>
+      </c>
+      <c r="D48" s="1">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A49" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B49" s="1">
+        <v>3.6017299999999998E-4</v>
+      </c>
+      <c r="C49" s="1">
+        <v>280</v>
+      </c>
+      <c r="D49" s="1">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A50" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B50" s="1">
+        <v>4.3636400000000001E-4</v>
+      </c>
+      <c r="C50" s="1">
+        <v>280</v>
+      </c>
+      <c r="D50" s="1">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A51" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B51" s="1">
+        <v>5.4891800000000002E-4</v>
+      </c>
+      <c r="C51" s="1">
+        <v>280</v>
+      </c>
+      <c r="D51" s="1">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A52" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B52" s="1">
+        <v>7.1515200000000004E-4</v>
+      </c>
+      <c r="C52" s="1">
+        <v>280</v>
+      </c>
+      <c r="D52" s="1">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A53" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B53" s="1">
+        <v>1.0147190000000001E-3</v>
+      </c>
+      <c r="C53" s="1">
+        <v>280</v>
+      </c>
+      <c r="D53" s="1">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A54" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B54" s="1">
+        <v>1.4943720000000001E-3</v>
+      </c>
+      <c r="C54" s="1">
+        <v>280</v>
+      </c>
+      <c r="D54" s="1">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A55" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B55" s="1">
+        <v>2.5800900000000002E-4</v>
+      </c>
+      <c r="C55" s="1">
+        <v>280</v>
+      </c>
+      <c r="D55" s="1">
+        <v>0.15</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A56" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B56" s="1">
+        <v>2.90909E-4</v>
+      </c>
+      <c r="C56" s="1">
+        <v>280</v>
+      </c>
+      <c r="D56" s="1">
+        <v>0.15</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A57" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B57" s="1">
+        <v>3.3419899999999998E-4</v>
+      </c>
+      <c r="C57" s="1">
+        <v>280</v>
+      </c>
+      <c r="D57" s="1">
+        <v>0.15</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A58" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B58" s="1">
+        <v>3.9307399999999998E-4</v>
+      </c>
+      <c r="C58" s="1">
+        <v>280</v>
+      </c>
+      <c r="D58" s="1">
+        <v>0.15</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A59" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B59" s="1">
+        <v>4.7445899999999999E-4</v>
+      </c>
+      <c r="C59" s="1">
+        <v>280</v>
+      </c>
+      <c r="D59" s="1">
+        <v>0.15</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A60" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B60" s="1">
+        <v>5.9913399999999997E-4</v>
+      </c>
+      <c r="C60" s="1">
+        <v>280</v>
+      </c>
+      <c r="D60" s="1">
+        <v>0.15</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A61" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B61" s="1">
+        <v>7.7229399999999998E-4</v>
+      </c>
+      <c r="C61" s="1">
+        <v>280</v>
+      </c>
+      <c r="D61" s="1">
+        <v>0.15</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>3</v>
       </c>
       <c r="B62">
-        <v>5.3200000000000003E-4</v>
+        <v>1.0320349999999999E-3</v>
       </c>
       <c r="C62">
-        <v>160</v>
+        <v>280</v>
       </c>
       <c r="D62">
-        <v>0.2</v>
-      </c>
-      <c r="E62">
-        <v>0</v>
-      </c>
-      <c r="F62">
-        <v>0</v>
-      </c>
-      <c r="G62">
-        <v>1.858317E-3</v>
-      </c>
-      <c r="H62">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="63" spans="1:8" x14ac:dyDescent="0.25">
+        <v>0.15</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>3</v>
       </c>
       <c r="B63">
-        <v>6.8900000000000005E-4</v>
+        <v>1.314286E-3</v>
       </c>
       <c r="C63">
-        <v>160</v>
+        <v>280</v>
       </c>
       <c r="D63">
-        <v>0.2</v>
-      </c>
-      <c r="E63">
-        <v>0</v>
-      </c>
-      <c r="F63">
-        <v>0</v>
-      </c>
-      <c r="G63">
-        <v>1.541461E-3</v>
-      </c>
-      <c r="H63">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="64" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A64" t="s">
-        <v>3</v>
-      </c>
-      <c r="B64">
-        <v>1.281E-3</v>
-      </c>
-      <c r="C64">
-        <v>160</v>
-      </c>
-      <c r="D64">
-        <v>0.2</v>
-      </c>
-      <c r="E64">
-        <v>0</v>
-      </c>
-      <c r="F64">
-        <v>0</v>
-      </c>
-      <c r="G64">
-        <v>1.2030529999999999E-3</v>
-      </c>
-      <c r="H64">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="65" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A65" t="s">
-        <v>3</v>
-      </c>
-      <c r="B65">
-        <v>2.52E-4</v>
-      </c>
-      <c r="C65">
-        <v>200</v>
-      </c>
-      <c r="D65">
-        <v>0.2</v>
-      </c>
-      <c r="E65">
-        <v>0</v>
-      </c>
-      <c r="F65">
-        <v>0</v>
-      </c>
-      <c r="G65">
-        <v>2.27729E-4</v>
-      </c>
-      <c r="H65">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="66" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A66" t="s">
-        <v>3</v>
-      </c>
-      <c r="B66">
-        <v>2.8299999999999999E-4</v>
-      </c>
-      <c r="C66">
-        <v>200</v>
-      </c>
-      <c r="D66">
-        <v>0.2</v>
-      </c>
-      <c r="E66">
-        <v>0</v>
-      </c>
-      <c r="F66">
-        <v>0</v>
-      </c>
-      <c r="G66">
-        <v>1.347741E-3</v>
-      </c>
-      <c r="H66">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="67" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A67" t="s">
-        <v>3</v>
-      </c>
-      <c r="B67">
-        <v>3.2499999999999999E-4</v>
-      </c>
-      <c r="C67">
-        <v>200</v>
-      </c>
-      <c r="D67">
-        <v>0.2</v>
-      </c>
-      <c r="E67">
-        <v>0</v>
-      </c>
-      <c r="F67">
-        <v>0</v>
-      </c>
-      <c r="G67">
-        <v>1.48168E-3</v>
-      </c>
-      <c r="H67">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="68" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A68" t="s">
-        <v>3</v>
-      </c>
-      <c r="B68">
-        <v>3.8299999999999999E-4</v>
-      </c>
-      <c r="C68">
-        <v>200</v>
-      </c>
-      <c r="D68">
-        <v>0.2</v>
-      </c>
-      <c r="E68">
-        <v>0</v>
-      </c>
-      <c r="F68">
-        <v>0</v>
-      </c>
-      <c r="G68">
-        <v>1.5823530000000001E-3</v>
-      </c>
-      <c r="H68">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="69" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A69" t="s">
-        <v>3</v>
-      </c>
-      <c r="B69">
-        <v>4.64E-4</v>
-      </c>
-      <c r="C69">
-        <v>200</v>
-      </c>
-      <c r="D69">
-        <v>0.2</v>
-      </c>
-      <c r="E69">
-        <v>0</v>
-      </c>
-      <c r="F69">
-        <v>0</v>
-      </c>
-      <c r="G69">
-        <v>1.264077E-3</v>
-      </c>
-      <c r="H69">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="70" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A70" t="s">
-        <v>3</v>
-      </c>
-      <c r="B70">
-        <v>5.8399999999999999E-4</v>
-      </c>
-      <c r="C70">
-        <v>200</v>
-      </c>
-      <c r="D70">
-        <v>0.2</v>
-      </c>
-      <c r="E70">
-        <v>0</v>
-      </c>
-      <c r="F70">
-        <v>0</v>
-      </c>
-      <c r="G70">
-        <v>1.7501089999999999E-3</v>
-      </c>
-      <c r="H70">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="71" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A71" t="s">
-        <v>3</v>
-      </c>
-      <c r="B71">
-        <v>7.8799999999999996E-4</v>
-      </c>
-      <c r="C71">
-        <v>200</v>
-      </c>
-      <c r="D71">
-        <v>0.2</v>
-      </c>
-      <c r="E71">
-        <v>0</v>
-      </c>
-      <c r="F71">
-        <v>0</v>
-      </c>
-      <c r="G71">
-        <v>1.2385709999999999E-3</v>
-      </c>
-      <c r="H71">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="72" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A72" t="s">
-        <v>3</v>
-      </c>
-      <c r="B72">
-        <v>1.0950000000000001E-3</v>
-      </c>
-      <c r="C72">
-        <v>200</v>
-      </c>
-      <c r="D72">
-        <v>0.2</v>
-      </c>
-      <c r="E72">
-        <v>0</v>
-      </c>
-      <c r="F72">
-        <v>0</v>
-      </c>
-      <c r="G72">
-        <v>9.1166800000000003E-4</v>
-      </c>
-      <c r="H72">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="73" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A73" t="s">
-        <v>3</v>
-      </c>
-      <c r="B73">
-        <v>1.5E-3</v>
-      </c>
-      <c r="C73">
-        <v>200</v>
-      </c>
-      <c r="D73">
-        <v>0.2</v>
-      </c>
-      <c r="E73">
-        <v>0</v>
-      </c>
-      <c r="F73">
-        <v>0</v>
-      </c>
-      <c r="G73">
-        <v>4.5693399999999999E-4</v>
-      </c>
-      <c r="H73">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="74" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A74" t="s">
-        <v>3</v>
-      </c>
-      <c r="B74">
-        <v>2.7099999999999997E-4</v>
-      </c>
-      <c r="C74">
-        <v>240</v>
-      </c>
-      <c r="D74">
-        <v>0.2</v>
-      </c>
-      <c r="E74">
-        <v>0</v>
-      </c>
-      <c r="F74">
-        <v>0</v>
-      </c>
-      <c r="G74">
-        <v>5.6943599999999999E-4</v>
-      </c>
-      <c r="H74">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="75" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A75" t="s">
-        <v>3</v>
-      </c>
-      <c r="B75">
-        <v>2.9799999999999998E-4</v>
-      </c>
-      <c r="C75">
-        <v>240</v>
-      </c>
-      <c r="D75">
-        <v>0.2</v>
-      </c>
-      <c r="E75">
-        <v>0</v>
-      </c>
-      <c r="F75">
-        <v>0</v>
-      </c>
-      <c r="G75">
-        <v>1.764112E-3</v>
-      </c>
-      <c r="H75">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="76" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A76" t="s">
-        <v>3</v>
-      </c>
-      <c r="B76">
-        <v>3.4299999999999999E-4</v>
-      </c>
-      <c r="C76">
-        <v>240</v>
-      </c>
-      <c r="D76">
-        <v>0.2</v>
-      </c>
-      <c r="E76">
-        <v>0</v>
-      </c>
-      <c r="F76">
-        <v>0</v>
-      </c>
-      <c r="G76">
-        <v>2.7815829999999998E-3</v>
-      </c>
-      <c r="H76">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="77" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A77" t="s">
-        <v>3</v>
-      </c>
-      <c r="B77">
-        <v>4.0400000000000001E-4</v>
-      </c>
-      <c r="C77">
-        <v>240</v>
-      </c>
-      <c r="D77">
-        <v>0.2</v>
-      </c>
-      <c r="E77">
-        <v>0</v>
-      </c>
-      <c r="F77">
-        <v>0</v>
-      </c>
-      <c r="G77">
-        <v>3.124384E-3</v>
-      </c>
-      <c r="H77">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="78" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A78" t="s">
-        <v>3</v>
-      </c>
-      <c r="B78">
-        <v>5.0299999999999997E-4</v>
-      </c>
-      <c r="C78">
-        <v>240</v>
-      </c>
-      <c r="D78">
-        <v>0.2</v>
-      </c>
-      <c r="E78">
-        <v>0</v>
-      </c>
-      <c r="F78">
-        <v>0</v>
-      </c>
-      <c r="G78">
-        <v>3.5047860000000002E-3</v>
-      </c>
-      <c r="H78">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="79" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A79" t="s">
-        <v>3</v>
-      </c>
-      <c r="B79">
-        <v>6.0999999999999997E-4</v>
-      </c>
-      <c r="C79">
-        <v>240</v>
-      </c>
-      <c r="D79">
-        <v>0.2</v>
-      </c>
-      <c r="E79">
-        <v>0</v>
-      </c>
-      <c r="F79">
-        <v>0</v>
-      </c>
-      <c r="G79">
-        <v>3.015471E-3</v>
-      </c>
-      <c r="H79">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="80" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A80" t="s">
-        <v>3</v>
-      </c>
-      <c r="B80">
-        <v>8.0400000000000003E-4</v>
-      </c>
-      <c r="C80">
-        <v>240</v>
-      </c>
-      <c r="D80">
-        <v>0.2</v>
-      </c>
-      <c r="E80">
-        <v>0</v>
-      </c>
-      <c r="F80">
-        <v>0</v>
-      </c>
-      <c r="G80">
-        <v>2.3056370000000001E-3</v>
-      </c>
-      <c r="H80">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="81" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A81" t="s">
-        <v>3</v>
-      </c>
-      <c r="B81">
-        <v>1.0920000000000001E-3</v>
-      </c>
-      <c r="C81">
-        <v>240</v>
-      </c>
-      <c r="D81">
-        <v>0.2</v>
-      </c>
-      <c r="E81">
-        <v>0</v>
-      </c>
-      <c r="F81">
-        <v>0</v>
-      </c>
-      <c r="G81">
-        <v>1.8617429999999999E-3</v>
-      </c>
-      <c r="H81">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="82" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A82" t="s">
-        <v>3</v>
-      </c>
-      <c r="B82">
-        <v>1.4159999999999999E-3</v>
-      </c>
-      <c r="C82">
-        <v>240</v>
-      </c>
-      <c r="D82">
-        <v>0.2</v>
-      </c>
-      <c r="E82">
-        <v>0</v>
-      </c>
-      <c r="F82">
-        <v>0</v>
-      </c>
-      <c r="G82">
-        <v>9.7170399999999999E-4</v>
-      </c>
-      <c r="H82">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="83" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A83" t="s">
-        <v>3</v>
-      </c>
-      <c r="B83">
-        <v>2.5399999999999999E-4</v>
-      </c>
-      <c r="C83">
-        <v>280</v>
-      </c>
-      <c r="D83">
-        <v>0.2</v>
-      </c>
-      <c r="E83">
-        <v>0</v>
-      </c>
-      <c r="F83">
-        <v>0</v>
-      </c>
-      <c r="G83">
-        <v>6.6906099999999998E-4</v>
-      </c>
-      <c r="H83">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="84" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A84" t="s">
-        <v>3</v>
-      </c>
-      <c r="B84">
-        <v>2.9399999999999999E-4</v>
-      </c>
-      <c r="C84">
-        <v>280</v>
-      </c>
-      <c r="D84">
-        <v>0.2</v>
-      </c>
-      <c r="E84">
-        <v>0</v>
-      </c>
-      <c r="F84">
-        <v>0</v>
-      </c>
-      <c r="G84">
-        <v>2.4819130000000001E-3</v>
-      </c>
-      <c r="H84">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="85" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A85" t="s">
-        <v>3</v>
-      </c>
-      <c r="B85">
-        <v>3.3700000000000001E-4</v>
-      </c>
-      <c r="C85">
-        <v>280</v>
-      </c>
-      <c r="D85">
-        <v>0.2</v>
-      </c>
-      <c r="E85">
-        <v>0</v>
-      </c>
-      <c r="F85">
-        <v>0</v>
-      </c>
-      <c r="G85">
-        <v>3.5047860000000002E-3</v>
-      </c>
-      <c r="H85">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="86" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A86" t="s">
-        <v>3</v>
-      </c>
-      <c r="B86">
-        <v>4.0200000000000001E-4</v>
-      </c>
-      <c r="C86">
-        <v>280</v>
-      </c>
-      <c r="D86">
-        <v>0.2</v>
-      </c>
-      <c r="E86">
-        <v>0</v>
-      </c>
-      <c r="F86">
-        <v>0</v>
-      </c>
-      <c r="G86">
-        <v>3.5300269999999998E-3</v>
-      </c>
-      <c r="H86">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="87" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A87" t="s">
-        <v>3</v>
-      </c>
-      <c r="B87">
-        <v>4.9700000000000005E-4</v>
-      </c>
-      <c r="C87">
-        <v>280</v>
-      </c>
-      <c r="D87">
-        <v>0.2</v>
-      </c>
-      <c r="E87">
-        <v>0</v>
-      </c>
-      <c r="F87">
-        <v>0</v>
-      </c>
-      <c r="G87">
-        <v>3.7511160000000001E-3</v>
-      </c>
-      <c r="H87">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="88" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A88" t="s">
-        <v>3</v>
-      </c>
-      <c r="B88">
-        <v>6.1700000000000004E-4</v>
-      </c>
-      <c r="C88">
-        <v>280</v>
-      </c>
-      <c r="D88">
-        <v>0.2</v>
-      </c>
-      <c r="E88">
-        <v>0</v>
-      </c>
-      <c r="F88">
-        <v>0</v>
-      </c>
-      <c r="G88">
-        <v>3.7918209999999999E-3</v>
-      </c>
-      <c r="H88">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="89" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A89" t="s">
-        <v>3</v>
-      </c>
-      <c r="B89">
-        <v>8.0000000000000004E-4</v>
-      </c>
-      <c r="C89">
-        <v>280</v>
-      </c>
-      <c r="D89">
-        <v>0.2</v>
-      </c>
-      <c r="E89">
-        <v>0</v>
-      </c>
-      <c r="F89">
-        <v>0</v>
-      </c>
-      <c r="G89">
-        <v>2.9280959999999998E-3</v>
-      </c>
-      <c r="H89">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="90" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A90" t="s">
-        <v>3</v>
-      </c>
-      <c r="B90">
-        <v>1.0989999999999999E-3</v>
-      </c>
-      <c r="C90">
-        <v>280</v>
-      </c>
-      <c r="D90">
-        <v>0.2</v>
-      </c>
-      <c r="E90">
-        <v>0</v>
-      </c>
-      <c r="F90">
-        <v>0</v>
-      </c>
-      <c r="G90">
-        <v>2.4002030000000001E-3</v>
-      </c>
-      <c r="H90">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="91" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A91" t="s">
-        <v>3</v>
-      </c>
-      <c r="B91">
-        <v>1.2780000000000001E-3</v>
-      </c>
-      <c r="C91">
-        <v>280</v>
-      </c>
-      <c r="D91">
-        <v>0.2</v>
-      </c>
-      <c r="E91">
-        <v>0</v>
-      </c>
-      <c r="F91">
-        <v>0</v>
-      </c>
-      <c r="G91">
-        <v>1.534342E-3</v>
-      </c>
-      <c r="H91">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="92" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A92" t="s">
-        <v>4</v>
-      </c>
-      <c r="B92">
-        <v>6.9999999999999999E-4</v>
-      </c>
-      <c r="C92">
-        <v>2050</v>
-      </c>
-      <c r="D92">
-        <v>0.3</v>
-      </c>
-      <c r="E92">
-        <v>0</v>
-      </c>
-      <c r="F92">
-        <v>0</v>
-      </c>
-      <c r="G92">
-        <v>5.9087439999999996E-3</v>
-      </c>
-      <c r="H92">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="93" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A93" t="s">
-        <v>4</v>
-      </c>
-      <c r="B93">
-        <v>9.0499999999999999E-4</v>
-      </c>
-      <c r="C93">
-        <v>2350</v>
-      </c>
-      <c r="D93">
-        <v>0.5</v>
-      </c>
-      <c r="E93">
-        <v>0</v>
-      </c>
-      <c r="F93">
-        <v>0</v>
-      </c>
-      <c r="G93">
-        <v>5.9087439999999996E-3</v>
-      </c>
-      <c r="H93">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="94" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A94" t="s">
-        <v>5</v>
-      </c>
-      <c r="B94">
-        <v>6.3250000000000003E-4</v>
-      </c>
-      <c r="C94">
-        <v>1600</v>
-      </c>
-      <c r="D94">
-        <v>0.3</v>
-      </c>
-      <c r="E94">
-        <v>0</v>
-      </c>
-      <c r="F94">
-        <v>0</v>
-      </c>
-      <c r="G94">
-        <v>5.9087439999999996E-3</v>
-      </c>
-      <c r="H94">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="95" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A95" t="s">
-        <v>5</v>
-      </c>
-      <c r="B95">
-        <v>6.0749999999999997E-4</v>
-      </c>
-      <c r="C95">
-        <v>1500</v>
-      </c>
-      <c r="D95">
-        <v>0.3</v>
-      </c>
-      <c r="E95">
-        <v>0</v>
-      </c>
-      <c r="F95">
-        <v>0</v>
-      </c>
-      <c r="G95">
-        <v>5.9087439999999996E-3</v>
-      </c>
-      <c r="H95">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="96" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A96" t="s">
-        <v>5</v>
-      </c>
-      <c r="B96">
-        <v>7.3800000000000005E-4</v>
-      </c>
-      <c r="C96">
-        <v>1450</v>
-      </c>
-      <c r="D96">
-        <v>0.5</v>
-      </c>
-      <c r="E96">
-        <v>0</v>
-      </c>
-      <c r="F96">
-        <v>0</v>
-      </c>
-      <c r="G96">
-        <v>5.9087439999999996E-3</v>
-      </c>
-      <c r="H96">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="97" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A97" t="s">
-        <v>5</v>
-      </c>
-      <c r="B97">
-        <v>8.6499999999999999E-4</v>
-      </c>
-      <c r="C97">
-        <v>1850</v>
-      </c>
-      <c r="D97">
-        <v>0.5</v>
-      </c>
-      <c r="E97">
-        <v>0</v>
-      </c>
-      <c r="F97">
-        <v>0</v>
-      </c>
-      <c r="G97">
-        <v>5.9087439999999996E-3</v>
-      </c>
-      <c r="H97">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="98" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A98" t="s">
-        <v>6</v>
-      </c>
-      <c r="B98">
-        <v>6.2750000000000002E-4</v>
-      </c>
-      <c r="C98">
-        <v>1600</v>
-      </c>
-      <c r="D98">
-        <v>0.3</v>
-      </c>
-      <c r="E98">
-        <v>0</v>
-      </c>
-      <c r="F98">
-        <v>0</v>
-      </c>
-      <c r="G98">
-        <v>5.9087439999999996E-3</v>
-      </c>
-      <c r="H98">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="99" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A99" t="s">
-        <v>6</v>
-      </c>
-      <c r="B99">
-        <v>5.8500000000000002E-4</v>
-      </c>
-      <c r="C99">
-        <v>1450</v>
-      </c>
-      <c r="D99">
-        <v>0.3</v>
-      </c>
-      <c r="E99">
-        <v>0</v>
-      </c>
-      <c r="F99">
-        <v>0</v>
-      </c>
-      <c r="G99">
-        <v>5.9087439999999996E-3</v>
-      </c>
-      <c r="H99">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="100" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A100" t="s">
-        <v>6</v>
-      </c>
-      <c r="B100">
-        <v>7.0750000000000001E-4</v>
-      </c>
-      <c r="C100">
-        <v>1400</v>
-      </c>
-      <c r="D100">
-        <v>0.5</v>
-      </c>
-      <c r="E100">
-        <v>0</v>
-      </c>
-      <c r="F100">
-        <v>0</v>
-      </c>
-      <c r="G100">
-        <v>5.9087439999999996E-3</v>
-      </c>
-      <c r="H100">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="101" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A101" t="s">
-        <v>6</v>
-      </c>
-      <c r="B101">
-        <v>6.3500000000000004E-4</v>
-      </c>
-      <c r="C101">
-        <v>1150</v>
-      </c>
-      <c r="D101">
-        <v>0.5</v>
-      </c>
-      <c r="E101">
-        <v>0</v>
-      </c>
-      <c r="F101">
-        <v>0</v>
-      </c>
-      <c r="G101">
-        <v>5.9087439999999996E-3</v>
-      </c>
-      <c r="H101">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="102" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A102" t="s">
-        <v>7</v>
-      </c>
-      <c r="B102">
-        <v>6.6750000000000002E-4</v>
-      </c>
-      <c r="C102">
-        <v>1600</v>
-      </c>
-      <c r="D102">
-        <v>0.3</v>
-      </c>
-      <c r="E102">
-        <v>0</v>
-      </c>
-      <c r="F102">
-        <v>0</v>
-      </c>
-      <c r="G102">
-        <v>5.9087439999999996E-3</v>
-      </c>
-      <c r="H102">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="103" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A103" t="s">
-        <v>7</v>
-      </c>
-      <c r="B103">
-        <v>6.3029999999999998E-4</v>
-      </c>
-      <c r="C103">
-        <v>1500</v>
-      </c>
-      <c r="D103">
-        <v>0.3</v>
-      </c>
-      <c r="E103">
-        <v>0</v>
-      </c>
-      <c r="F103">
-        <v>0</v>
-      </c>
-      <c r="G103">
-        <v>5.9087439999999996E-3</v>
-      </c>
-      <c r="H103">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="104" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A104" t="s">
-        <v>7</v>
-      </c>
-      <c r="B104">
-        <v>7.2250000000000005E-4</v>
-      </c>
-      <c r="C104">
-        <v>1350</v>
-      </c>
-      <c r="D104">
-        <v>0.5</v>
-      </c>
-      <c r="E104">
-        <v>0</v>
-      </c>
-      <c r="F104">
-        <v>0</v>
-      </c>
-      <c r="G104">
-        <v>5.9087439999999996E-3</v>
-      </c>
-      <c r="H104">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="105" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A105" t="s">
-        <v>7</v>
-      </c>
-      <c r="B105">
-        <v>6.7250000000000003E-4</v>
-      </c>
-      <c r="C105">
-        <v>1200</v>
-      </c>
-      <c r="D105">
-        <v>0.5</v>
-      </c>
-      <c r="E105">
-        <v>0</v>
-      </c>
-      <c r="F105">
-        <v>0</v>
-      </c>
-      <c r="G105">
-        <v>5.9087439999999996E-3</v>
-      </c>
-      <c r="H105">
-        <v>0</v>
+        <v>0.15</v>
       </c>
     </row>
   </sheetData>

</xml_diff>